<commit_message>
feat(fw): first firmware with .ioc config
CubeIDE project was add including pin config from excel in fw carpet
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robocup\Documents\pinpon\Phoenix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB64457B-026D-4AF7-9499-D48D63889510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{FB64457B-026D-4AF7-9499-D48D63889510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA603779-0DA2-4A9F-908E-474CD6B29F00}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +186,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,21 +215,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -263,21 +304,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="P5:U25" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="P5:U26" totalsRowCount="1">
   <autoFilter ref="P5:U25" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2A8164C2-2FB7-4C23-97F1-2EB7091D5D63}" name="COMPONENTES"/>
-    <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="7" totalsRowDxfId="3">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F8E4DDA3-B94B-4AA6-A9F3-1C390E031E27}" name="Link" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{F8E4DDA3-B94B-4AA6-A9F3-1C390E031E27}" name="Link" dataDxfId="6" totalsRowDxfId="2">
       <calculatedColumnFormula>HYPERLINK("https://github.com/tu_repo","Ver repo")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3EB6D48B-B456-4C54-9366-899F34DB475D}" name="Precio unitario(USD)"/>
-    <tableColumn id="5" xr3:uid="{E2B14899-0F61-4692-90A3-AC74A17D725D}" name="TOTAL(USD)" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{E2B14899-0F61-4692-90A3-AC74A17D725D}" name="TOTAL(USD)" dataDxfId="5" totalsRowDxfId="1">
       <calculatedColumnFormula>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{81E0CD81-31E1-4B12-A1CA-8459D81315C8}" name="TOTAL(CLP)" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{81E0CD81-31E1-4B12-A1CA-8459D81315C8}" name="TOTAL(CLP)" dataDxfId="4" totalsRowDxfId="0" totalsRowCellStyle="Moneda [0]">
       <calculatedColumnFormula>PRODUCT(Tabla2[[#This Row],[TOTAL(USD)]],941.85)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -602,43 +643,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
-  <dimension ref="A3:U25"/>
+  <dimension ref="A3:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" topLeftCell="M4" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1"/>
-    <col min="19" max="19" width="21.42578125" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.5546875" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
+    <col min="17" max="17" width="13.88671875" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" customWidth="1"/>
+    <col min="19" max="19" width="21.44140625" customWidth="1"/>
+    <col min="20" max="20" width="13.5546875" customWidth="1"/>
+    <col min="21" max="21" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -688,7 +729,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -721,7 +762,7 @@
         <v>847.66500000000008</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -754,7 +795,7 @@
         <v>395.577</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -774,7 +815,6 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>4</v>
       </c>
-      <c r="R8" s="2"/>
       <c r="T8">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>4</v>
@@ -784,7 +824,7 @@
         <v>3767.4</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -801,7 +841,6 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="R9" s="2"/>
       <c r="T9">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1</v>
@@ -811,7 +850,7 @@
         <v>941.85</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -844,7 +883,7 @@
         <v>320.22900000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>17</v>
       </c>
@@ -874,7 +913,7 @@
         <v>226.04400000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>18</v>
       </c>
@@ -907,7 +946,7 @@
         <v>602.78399999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>19</v>
       </c>
@@ -937,7 +976,7 @@
         <v>414.41399999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>22</v>
       </c>
@@ -951,7 +990,7 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="R14" s="3" t="str">
+      <c r="R14" s="2" t="str">
         <f>HYPERLINK("https://mou.sr/43wYwnr","Mouser")</f>
         <v>Mouser</v>
       </c>
@@ -967,7 +1006,7 @@
         <v>339.06599999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>20</v>
       </c>
@@ -997,7 +1036,7 @@
         <v>6272.7210000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1066,7 @@
         <v>1695.33</v>
       </c>
     </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>23</v>
       </c>
@@ -1057,7 +1096,7 @@
         <v>960.68700000000001</v>
       </c>
     </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>24</v>
       </c>
@@ -1071,7 +1110,6 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
-      <c r="R18" s="2"/>
       <c r="T18">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>3</v>
@@ -1081,7 +1119,7 @@
         <v>2825.55</v>
       </c>
     </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>25</v>
       </c>
@@ -1111,7 +1149,7 @@
         <v>282.55500000000006</v>
       </c>
     </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>26</v>
       </c>
@@ -1125,7 +1163,6 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="R20" s="2"/>
       <c r="T20">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>2</v>
@@ -1135,7 +1172,7 @@
         <v>1883.7</v>
       </c>
     </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>27</v>
       </c>
@@ -1149,7 +1186,6 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="R21" s="2"/>
       <c r="T21">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>2</v>
@@ -1159,7 +1195,7 @@
         <v>1883.7</v>
       </c>
     </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>29</v>
       </c>
@@ -1189,7 +1225,7 @@
         <v>9041.760000000002</v>
       </c>
     </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>31</v>
       </c>
@@ -1203,7 +1239,7 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="R23" s="3" t="str">
+      <c r="R23" s="2" t="str">
         <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
         <v>Mouser</v>
       </c>
@@ -1219,7 +1255,7 @@
         <v>94.185000000000002</v>
       </c>
     </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>32</v>
       </c>
@@ -1236,7 +1272,7 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="R24" s="3" t="str">
+      <c r="R24" s="2" t="str">
         <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
         <v>Mouser</v>
       </c>
@@ -1252,7 +1288,7 @@
         <v>188.37</v>
       </c>
     </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>33</v>
       </c>
@@ -1266,7 +1302,6 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="R25" s="2"/>
       <c r="T25">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>2</v>
@@ -1275,6 +1310,12 @@
         <f>PRODUCT(Tabla2[[#This Row],[TOTAL(USD)]],941.85)</f>
         <v>1883.7</v>
       </c>
+    </row>
+    <row r="26" spans="5:21" x14ac:dyDescent="0.3">
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
docs(rev1 - Passive components)
primera revision de documento de elementos pasivos, se deja en "x" componentes que faltan revisar y acrualizar link de MOUSER
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1Principal\USM\2025 -2\Diseño\PC1_v3\phoenix-c1-\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1Principal\USM\2025 -2\DEE\PC1_v3\phoenix-c1-\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618450D5-53B4-48AB-AFC8-596F7511678E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>power input</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>TOTAL(CLP)~</t>
+  </si>
+  <si>
+    <t>DANGER</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -225,7 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -234,22 +240,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -329,6 +319,16 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{308D2B94-B45D-41E6-8288-C856D97EC24C}" name="Tabla4" displayName="Tabla4" ref="O5:O25" totalsRowShown="0">
+  <autoFilter ref="O5:O25" xr:uid="{308D2B94-B45D-41E6-8288-C856D97EC24C}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{FAC6BF7B-01EC-4986-A1BE-12FA75B22E70}" name="DANGER"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
   <dimension ref="A2:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,6 +667,7 @@
     <col min="11" max="11" width="16.109375" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="18.5546875" customWidth="1"/>
+    <col min="15" max="15" width="11.77734375" customWidth="1"/>
     <col min="16" max="16" width="17.44140625" customWidth="1"/>
     <col min="17" max="17" width="13.88671875" customWidth="1"/>
     <col min="18" max="18" width="8.88671875" customWidth="1"/>
@@ -689,11 +690,11 @@
       </c>
       <c r="T3">
         <f>SUM(Tabla2[CantX$(USD)])</f>
-        <v>27.620000000000005</v>
+        <v>28.340000000000003</v>
       </c>
       <c r="U3">
         <f>ROUND(SUM(Tabla2[CantX$(CLP)]),0)</f>
-        <v>26014</v>
+        <v>26692</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -732,6 +733,9 @@
       <c r="L5" t="s">
         <v>30</v>
       </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
       <c r="P5" t="s">
         <v>13</v>
       </c>
@@ -838,19 +842,19 @@
         <v>4</v>
       </c>
       <c r="R8" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47sd9K6","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="S8">
-        <v>0.16</v>
+        <v>0.34</v>
       </c>
       <c r="T8">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.64</v>
+        <v>1.36</v>
       </c>
       <c r="U8">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>602.78399999999999</v>
+        <v>1280.9160000000002</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -1019,6 +1023,9 @@
       <c r="G14">
         <v>2</v>
       </c>
+      <c r="O14" t="s">
+        <v>46</v>
+      </c>
       <c r="P14" t="s">
         <v>22</v>
       </c>
@@ -1139,6 +1146,9 @@
       <c r="I18">
         <v>3</v>
       </c>
+      <c r="O18" t="s">
+        <v>46</v>
+      </c>
       <c r="P18" t="s">
         <v>24</v>
       </c>
@@ -1177,7 +1187,7 @@
         <v>3</v>
       </c>
       <c r="R19" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/4hu3MOB","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="S19">
@@ -1199,6 +1209,9 @@
       <c r="J20">
         <v>2</v>
       </c>
+      <c r="O20" t="s">
+        <v>46</v>
+      </c>
       <c r="P20" t="s">
         <v>26</v>
       </c>
@@ -1229,6 +1242,9 @@
       <c r="J21">
         <v>2</v>
       </c>
+      <c r="O21" t="s">
+        <v>46</v>
+      </c>
       <c r="P21" t="s">
         <v>40</v>
       </c>
@@ -1289,6 +1305,9 @@
       <c r="L23">
         <v>1</v>
       </c>
+      <c r="O23" t="s">
+        <v>46</v>
+      </c>
       <c r="P23" t="s">
         <v>31</v>
       </c>
@@ -1322,6 +1341,9 @@
       <c r="L24">
         <v>1</v>
       </c>
+      <c r="O24" t="s">
+        <v>46</v>
+      </c>
       <c r="P24" t="s">
         <v>32</v>
       </c>
@@ -1352,6 +1374,9 @@
       <c r="L25">
         <v>2</v>
       </c>
+      <c r="O25" t="s">
+        <v>46</v>
+      </c>
       <c r="P25" t="s">
         <v>33</v>
       </c>
@@ -1381,10 +1406,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(schematics): schematic for bulk capacitance was finished
More passive components has been add. it was added component for LED sense and Datasheet for components was added too.
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{391201DB-6E02-4244-9B41-11C928A02FBB}"/>
+  <xr:revisionPtr revIDLastSave="306" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E641EB0-0220-4BB3-AD76-29541092022D}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="2145" windowWidth="21600" windowHeight="11235" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Componentes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="91">
   <si>
     <t>power input</t>
   </si>
@@ -202,12 +202,6 @@
   </si>
   <si>
     <t>TPN19008QM,LQ</t>
-  </si>
-  <si>
-    <t>Voltage Max</t>
-  </si>
-  <si>
-    <t>Voltaje</t>
   </si>
   <si>
     <t>CSSH0805FT2L00</t>
@@ -321,6 +315,33 @@
   </si>
   <si>
     <t>https://www.mouser.cl/ProductDetail/YAGEO/AF0402JR-072KL?qs=sGAEpiMZZMtlubZbdhIBIIzXXd8RXMQ1A4VeykjrMVQ%3D</t>
+  </si>
+  <si>
+    <t>C0603X473K1RACTU</t>
+  </si>
+  <si>
+    <t>1000pf 6.3V</t>
+  </si>
+  <si>
+    <t>08056C102JAT2A</t>
+  </si>
+  <si>
+    <t>RC0603JR-0722RL</t>
+  </si>
+  <si>
+    <t>1000pF</t>
+  </si>
+  <si>
+    <t>22 Ω</t>
+  </si>
+  <si>
+    <t>47uF 100V</t>
+  </si>
+  <si>
+    <t>RT0603BRD07560RL</t>
+  </si>
+  <si>
+    <t>APT1608SURC</t>
   </si>
 </sst>
 </file>
@@ -407,14 +428,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -447,6 +468,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -826,34 +851,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
   <dimension ref="A2:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" customWidth="1"/>
-    <col min="20" max="20" width="20.140625" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" customWidth="1"/>
+    <col min="20" max="20" width="20.109375" customWidth="1"/>
+    <col min="21" max="21" width="13.5546875" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="U2" t="s">
         <v>39</v>
       </c>
@@ -861,25 +886,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="U3">
         <f>SUM(Tabla2[CantX$(USD)])</f>
-        <v>22.790000000000003</v>
+        <v>30.19</v>
       </c>
       <c r="V3">
         <f>ROUND(SUM(Tabla2[CantX$(CLP)]),0)</f>
-        <v>21465</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+        <v>28435</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -914,13 +939,13 @@
         <v>13</v>
       </c>
       <c r="O5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R5" t="s">
         <v>37</v>
@@ -938,7 +963,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -955,7 +980,7 @@
         <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R6">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -977,7 +1002,7 @@
         <v>320.22900000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -994,7 +1019,7 @@
         <v>20</v>
       </c>
       <c r="P7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R7">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1016,7 +1041,7 @@
         <v>1045.4535000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +1061,7 @@
         <v>14</v>
       </c>
       <c r="P8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R8">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1058,7 +1083,7 @@
         <v>3391.2000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1069,11 +1094,16 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>83</v>
+      </c>
+      <c r="O9" t="s">
+        <v>84</v>
+      </c>
+      <c r="P9" t="s">
+        <v>63</v>
       </c>
       <c r="R9">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S9" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
@@ -1084,14 +1114,14 @@
       </c>
       <c r="U9">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="V9">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>94.185000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+        <v>282.55500000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1105,10 +1135,10 @@
         <v>19</v>
       </c>
       <c r="O10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="P10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R10">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1130,7 +1160,7 @@
         <v>414.41399999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>17</v>
       </c>
@@ -1141,7 +1171,7 @@
         <v>31</v>
       </c>
       <c r="Q11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R11">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1163,7 +1193,7 @@
         <v>94.185000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>18</v>
       </c>
@@ -1177,10 +1207,10 @@
         <v>15</v>
       </c>
       <c r="O12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R12">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1202,7 +1232,7 @@
         <v>1582.308</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>19</v>
       </c>
@@ -1213,10 +1243,10 @@
         <v>17</v>
       </c>
       <c r="O13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R13">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1238,7 +1268,7 @@
         <v>226.04400000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>22</v>
       </c>
@@ -1246,13 +1276,13 @@
         <v>2</v>
       </c>
       <c r="N14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R14">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1274,7 +1304,7 @@
         <v>640.45800000000008</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>20</v>
       </c>
@@ -1285,10 +1315,10 @@
         <v>18</v>
       </c>
       <c r="O15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="P15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R15">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1310,7 +1340,7 @@
         <v>904.17600000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>21</v>
       </c>
@@ -1321,14 +1351,13 @@
         <v>29</v>
       </c>
       <c r="O16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R16">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="S16" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
@@ -1339,14 +1368,14 @@
       </c>
       <c r="U16">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>2.4000000000000004</v>
+        <v>9.6000000000000014</v>
       </c>
       <c r="V16">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>2260.4400000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="5:22" x14ac:dyDescent="0.25">
+        <v>9041.760000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>23</v>
       </c>
@@ -1357,7 +1386,7 @@
         <v>32</v>
       </c>
       <c r="Q17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R17">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1379,7 +1408,7 @@
         <v>282.55500000000006</v>
       </c>
     </row>
-    <row r="18" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>24</v>
       </c>
@@ -1409,7 +1438,7 @@
         <v>4492.6245000000008</v>
       </c>
     </row>
-    <row r="19" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>25</v>
       </c>
@@ -1439,7 +1468,7 @@
         <v>960.68700000000001</v>
       </c>
     </row>
-    <row r="20" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>26</v>
       </c>
@@ -1450,7 +1479,7 @@
         <v>21</v>
       </c>
       <c r="P20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R20">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1472,7 +1501,7 @@
         <v>1130.22</v>
       </c>
     </row>
-    <row r="21" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>27</v>
       </c>
@@ -1483,17 +1512,17 @@
         <v>22</v>
       </c>
       <c r="O21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R21">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="T21">
         <v>0.18</v>
@@ -1507,7 +1536,7 @@
         <v>339.06599999999997</v>
       </c>
     </row>
-    <row r="22" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>29</v>
       </c>
@@ -1517,8 +1546,11 @@
       <c r="N22" t="s">
         <v>24</v>
       </c>
-      <c r="Q22" t="s">
-        <v>65</v>
+      <c r="O22" t="s">
+        <v>85</v>
+      </c>
+      <c r="P22" t="s">
+        <v>63</v>
       </c>
       <c r="R22">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1540,7 +1572,7 @@
         <v>1695.33</v>
       </c>
     </row>
-    <row r="23" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>31</v>
       </c>
@@ -1550,8 +1582,11 @@
       <c r="N23" t="s">
         <v>26</v>
       </c>
-      <c r="Q23" t="s">
-        <v>65</v>
+      <c r="O23" t="s">
+        <v>89</v>
+      </c>
+      <c r="P23" t="s">
+        <v>63</v>
       </c>
       <c r="R23">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1573,7 +1608,7 @@
         <v>216.62550000000002</v>
       </c>
     </row>
-    <row r="24" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>32</v>
       </c>
@@ -1586,8 +1621,11 @@
       <c r="N24" t="s">
         <v>40</v>
       </c>
-      <c r="Q24" t="s">
-        <v>65</v>
+      <c r="O24" t="s">
+        <v>90</v>
+      </c>
+      <c r="P24" t="s">
+        <v>63</v>
       </c>
       <c r="R24">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1609,7 +1647,7 @@
         <v>772.31700000000001</v>
       </c>
     </row>
-    <row r="25" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>33</v>
       </c>
@@ -1620,7 +1658,7 @@
         <v>33</v>
       </c>
       <c r="Q25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R25">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1642,11 +1680,11 @@
         <v>602.78399999999999</v>
       </c>
     </row>
-    <row r="26" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:22" x14ac:dyDescent="0.3">
       <c r="V26" s="3"/>
     </row>
-    <row r="27" spans="5:22" x14ac:dyDescent="0.25">
-      <c r="R27" s="8"/>
+    <row r="27" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="R27" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1664,317 +1702,406 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EDAD98-4A51-48B0-BAE4-039E551A8C8C}">
-  <dimension ref="B2:I31"/>
+  <dimension ref="B2:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I4" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
       </c>
       <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>63</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>54</v>
       </c>
       <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>61</v>
-      </c>
-      <c r="C20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>63</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
         <v>62</v>
       </c>
-      <c r="C26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" t="s">
-        <v>82</v>
+      <c r="E35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(schematic): schematic for smt32g4 was finished
More passive components was added to the excel and altium and .BomDom was created
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="306" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E641EB0-0220-4BB3-AD76-29541092022D}"/>
+  <xr:revisionPtr revIDLastSave="400" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{876206C4-3322-4CF9-8CEB-7A5A5BEA836D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="108">
   <si>
     <t>power input</t>
   </si>
@@ -342,6 +342,57 @@
   </si>
   <si>
     <t>APT1608SURC</t>
+  </si>
+  <si>
+    <t>RC0603FR-104K7L</t>
+  </si>
+  <si>
+    <t>https://www.mouser.cl/ProductDetail/YAGEO/RC0603FR-104K7L?qs=sGAEpiMZZMtlubZbdhIBIHvQf5egq9lv0mk7h5hs6B0%3D</t>
+  </si>
+  <si>
+    <t>B82464P4333M000</t>
+  </si>
+  <si>
+    <t>3.3 uh</t>
+  </si>
+  <si>
+    <t>GRM022R60J104ME15L</t>
+  </si>
+  <si>
+    <t>GRM155R60J106ME05D</t>
+  </si>
+  <si>
+    <t>SMBJ48D-M3/I</t>
+  </si>
+  <si>
+    <t>10uF 6.3V</t>
+  </si>
+  <si>
+    <t>0.1uF 6.3V</t>
+  </si>
+  <si>
+    <t>4.7uF 6.3V</t>
+  </si>
+  <si>
+    <t>GRT033R60J104KE01J</t>
+  </si>
+  <si>
+    <t>0.1 uF 6.3 V</t>
+  </si>
+  <si>
+    <t>GRM188R60J105KA01D</t>
+  </si>
+  <si>
+    <t>GRM035R60J475ME15D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.cl/ProductDetail/Murata-Electronics/GRT033R60J104KE01J?qs=sGAEpiMZZMukHu%252BjC5l7YV930%2Fyx0fDoI9r4dHYiKoY%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.cl/ProductDetail/Murata-Electronics/GRM188R60J105KA01D?qs=dddcrN876Gomyq%2FPjh7oaA%3D%3D&amp;srsltid=AfmBOoo3DNiuM7aq0lB6KzkD8q2hbIrqvJvOPE08Ax-0afc0q3WD7aso</t>
+  </si>
+  <si>
+    <t>https://www.mouser.cl/ProductDetail/Murata-Electronics/GRM035R60J475ME15D?qs=I53XXhTNm8vhFCgPvCZ%252BPQ%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -441,9 +492,27 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -492,24 +561,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:V26" totalsRowCount="1">
-  <autoFilter ref="N5:V25" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:V29" totalsRowCount="1">
+  <autoFilter ref="N5:V28" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2A8164C2-2FB7-4C23-97F1-2EB7091D5D63}" name="COMPONENTES"/>
     <tableColumn id="9" xr3:uid="{916D2FE0-85EB-46DA-9799-D85CA8D5156F}" name="Part Number"/>
     <tableColumn id="8" xr3:uid="{B1046C3A-A1F3-421E-9436-C5BB3C6B237A}" name="Altium"/>
     <tableColumn id="7" xr3:uid="{ADE89E6D-F7FC-45CE-A5CB-99276119FEF7}" name="D"/>
-    <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="5" totalsRowDxfId="1">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F8E4DDA3-B94B-4AA6-A9F3-1C390E031E27}" name="Link" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F8E4DDA3-B94B-4AA6-A9F3-1C390E031E27}" name="Link" dataDxfId="4">
       <calculatedColumnFormula>HYPERLINK("https://github.com/tu_repo","Ver repo")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3EB6D48B-B456-4C54-9366-899F34DB475D}" name="Precio unitario(USD)"/>
-    <tableColumn id="5" xr3:uid="{E2B14899-0F61-4692-90A3-AC74A17D725D}" name="CantX$(USD)" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E2B14899-0F61-4692-90A3-AC74A17D725D}" name="CantX$(USD)" dataDxfId="3">
       <calculatedColumnFormula>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{81E0CD81-31E1-4B12-A1CA-8459D81315C8}" name="CantX$(CLP)" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="6" xr3:uid="{81E0CD81-31E1-4B12-A1CA-8459D81315C8}" name="CantX$(CLP)" dataDxfId="2" totalsRowDxfId="0">
       <calculatedColumnFormula>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -849,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
-  <dimension ref="A2:V27"/>
+  <dimension ref="A2:V29"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,10 +937,10 @@
     <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="17.44140625" customWidth="1"/>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" customWidth="1"/>
+    <col min="18" max="18" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.88671875" customWidth="1"/>
     <col min="20" max="20" width="20.109375" customWidth="1"/>
     <col min="21" max="21" width="13.5546875" customWidth="1"/>
@@ -892,11 +961,11 @@
       </c>
       <c r="U3">
         <f>SUM(Tabla2[CantX$(USD)])</f>
-        <v>30.19</v>
+        <v>36.869999999999997</v>
       </c>
       <c r="V3">
         <f>ROUND(SUM(Tabla2[CantX$(CLP)]),0)</f>
-        <v>28435</v>
+        <v>34727</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
@@ -1170,7 +1239,10 @@
       <c r="N11" t="s">
         <v>31</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="O11" t="s">
+        <v>95</v>
+      </c>
+      <c r="P11" t="s">
         <v>63</v>
       </c>
       <c r="R11">
@@ -1385,7 +1457,10 @@
       <c r="N17" t="s">
         <v>32</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="O17" t="s">
+        <v>96</v>
+      </c>
+      <c r="P17" t="s">
         <v>63</v>
       </c>
       <c r="R17">
@@ -1416,7 +1491,13 @@
         <v>3</v>
       </c>
       <c r="N18" t="s">
-        <v>35</v>
+        <v>94</v>
+      </c>
+      <c r="O18" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18" t="s">
+        <v>63</v>
       </c>
       <c r="R18">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
@@ -1448,6 +1529,12 @@
       <c r="N19" t="s">
         <v>36</v>
       </c>
+      <c r="O19" t="s">
+        <v>97</v>
+      </c>
+      <c r="P19" t="s">
+        <v>63</v>
+      </c>
       <c r="R19">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
@@ -1478,6 +1565,9 @@
       <c r="N20" t="s">
         <v>21</v>
       </c>
+      <c r="O20" t="s">
+        <v>55</v>
+      </c>
       <c r="P20" t="s">
         <v>63</v>
       </c>
@@ -1655,36 +1745,110 @@
         <v>2</v>
       </c>
       <c r="N25" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q25" t="s">
+        <v>102</v>
+      </c>
+      <c r="O25" t="s">
+        <v>101</v>
+      </c>
+      <c r="P25" t="s">
         <v>63</v>
       </c>
       <c r="R25">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>2</v>
-      </c>
-      <c r="S25" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47cQYJ1","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="T25">
-        <v>0.32</v>
+        <v>5</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="U25">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.64</v>
+        <v>5</v>
       </c>
       <c r="V25">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>602.78399999999999</v>
+        <v>4709.25</v>
       </c>
     </row>
     <row r="26" spans="5:22" x14ac:dyDescent="0.3">
-      <c r="V26" s="3"/>
+      <c r="N26" t="s">
+        <v>73</v>
+      </c>
+      <c r="O26" t="s">
+        <v>103</v>
+      </c>
+      <c r="P26" t="s">
+        <v>63</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="U26">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>941.85</v>
+      </c>
     </row>
     <row r="27" spans="5:22" x14ac:dyDescent="0.3">
-      <c r="R27" s="6"/>
+      <c r="N27" t="s">
+        <v>100</v>
+      </c>
+      <c r="O27" t="s">
+        <v>104</v>
+      </c>
+      <c r="P27" t="s">
+        <v>63</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="U27">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>941.85</v>
+      </c>
+    </row>
+    <row r="28" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P28" t="s">
+        <v>63</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="T28">
+        <v>0.32</v>
+      </c>
+      <c r="U28">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.32</v>
+      </c>
+      <c r="V28">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>301.392</v>
+      </c>
+    </row>
+    <row r="29" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="R29" s="6"/>
+      <c r="V29" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1702,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EDAD98-4A51-48B0-BAE4-039E551A8C8C}">
-  <dimension ref="B2:I36"/>
+  <dimension ref="B2:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2104,6 +2268,62 @@
         <v>46</v>
       </c>
     </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>

</xml_diff>

<commit_message>
docs(excel): Footprint checker was added to excel
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="400" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{876206C4-3322-4CF9-8CEB-7A5A5BEA836D}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EE91FA-2241-4505-AC8B-938DC92868D4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Componentes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="110">
   <si>
     <t>power input</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t>https://www.mouser.cl/ProductDetail/Murata-Electronics/GRM035R60J475ME15D?qs=I53XXhTNm8vhFCgPvCZ%252BPQ%3D%3D</t>
+  </si>
+  <si>
+    <t>PCBlibrary</t>
+  </si>
+  <si>
+    <t>FP Corregido</t>
   </si>
 </sst>
 </file>
@@ -561,12 +567,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:V29" totalsRowCount="1">
-  <autoFilter ref="N5:V28" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:X29" totalsRowCount="1">
+  <autoFilter ref="N5:X28" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{2A8164C2-2FB7-4C23-97F1-2EB7091D5D63}" name="COMPONENTES"/>
     <tableColumn id="9" xr3:uid="{916D2FE0-85EB-46DA-9799-D85CA8D5156F}" name="Part Number"/>
     <tableColumn id="8" xr3:uid="{B1046C3A-A1F3-421E-9436-C5BB3C6B237A}" name="Altium"/>
+    <tableColumn id="10" xr3:uid="{2CEA38F0-0C3D-417B-A37F-12BD902EBA47}" name="PCBlibrary"/>
+    <tableColumn id="11" xr3:uid="{F6CD5E74-C2A7-497A-977E-F83F137C4127}" name="FP Corregido"/>
     <tableColumn id="7" xr3:uid="{ADE89E6D-F7FC-45CE-A5CB-99276119FEF7}" name="D"/>
     <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="5" totalsRowDxfId="1">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</calculatedColumnFormula>
@@ -587,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}" name="Tabla3" displayName="Tabla3" ref="U2:V3" totalsRowShown="0">
-  <autoFilter ref="U2:V3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}" name="Tabla3" displayName="Tabla3" ref="W2:X3" totalsRowShown="0">
+  <autoFilter ref="W2:X3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6441C57D-BDB7-4FF4-9BC8-CECA7F77E429}" name="TOTAL(USD)">
       <calculatedColumnFormula>SUM(Tabla2[CantX$(USD)])</calculatedColumnFormula>
@@ -918,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
-  <dimension ref="A2:V29"/>
+  <dimension ref="A2:X29"/>
   <sheetViews>
-    <sheetView topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -939,41 +947,43 @@
     <col min="14" max="14" width="17.44140625" customWidth="1"/>
     <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" customWidth="1"/>
-    <col min="20" max="20" width="20.109375" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5546875" customWidth="1"/>
+    <col min="19" max="19" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.88671875" customWidth="1"/>
+    <col min="22" max="22" width="20.109375" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U2" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W2" t="s">
         <v>39</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <f>SUM(Tabla2[CantX$(USD)])</f>
         <v>36.869999999999997</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <f>ROUND(SUM(Tabla2[CantX$(CLP)]),0)</f>
         <v>34727</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1014,25 +1024,31 @@
         <v>70</v>
       </c>
       <c r="Q5" t="s">
+        <v>108</v>
+      </c>
+      <c r="R5" t="s">
+        <v>109</v>
+      </c>
+      <c r="S5" t="s">
         <v>61</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>37</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>38</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>41</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" t="s">
         <v>42</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1051,27 +1067,27 @@
       <c r="P6" t="s">
         <v>63</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="S6" s="1" t="str">
+      <c r="U6" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/42XoOiu","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>0.34</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.34</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>320.22900000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1090,27 +1106,27 @@
       <c r="P7" t="s">
         <v>63</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="S7" s="1" t="str">
+      <c r="U7" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3Jxp5Cd","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>1.1100000000000001</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>1045.4535000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1132,27 +1148,27 @@
       <c r="P8" t="s">
         <v>63</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>4</v>
       </c>
-      <c r="S8" s="1" t="str">
+      <c r="U8" s="1" t="str">
         <f>HYPERLINK("https://octopart.com/es/xt60pw-m-amass-118051292","Octopart")</f>
         <v>Octopart</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>0.9</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>3.6</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],942)</f>
         <v>3391.2000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1171,26 +1187,26 @@
       <c r="P9" t="s">
         <v>63</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>3</v>
       </c>
-      <c r="S9" s="1" t="str">
+      <c r="U9" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>0.1</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>282.55500000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1209,27 +1225,27 @@
       <c r="P10" t="s">
         <v>63</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="S10" s="1" t="str">
+      <c r="U10" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47aSprm","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>0.44</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.44</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>414.41399999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>17</v>
       </c>
@@ -1245,27 +1261,27 @@
       <c r="P11" t="s">
         <v>63</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="S11" s="2" t="str">
+      <c r="U11" s="2" t="str">
         <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>0.1</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.1</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>94.185000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>18</v>
       </c>
@@ -1284,27 +1300,27 @@
       <c r="P12" t="s">
         <v>63</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>4</v>
       </c>
-      <c r="S12" s="1" t="str">
+      <c r="U12" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/4oCNLrW","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>0.42</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.68</v>
       </c>
-      <c r="V12">
+      <c r="X12">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>1582.308</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>19</v>
       </c>
@@ -1320,27 +1336,27 @@
       <c r="P13" t="s">
         <v>63</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="S13" s="1" t="str">
+      <c r="U13" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/43ubkLk","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T13">
+      <c r="V13">
         <v>0.24</v>
       </c>
-      <c r="U13">
+      <c r="W13">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.24</v>
       </c>
-      <c r="V13">
+      <c r="X13">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>226.04400000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>22</v>
       </c>
@@ -1356,27 +1372,27 @@
       <c r="P14" t="s">
         <v>63</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="S14" s="1" t="str">
+      <c r="U14" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <v>0.34</v>
       </c>
-      <c r="U14">
+      <c r="W14">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.68</v>
       </c>
-      <c r="V14">
+      <c r="X14">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>640.45800000000008</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>20</v>
       </c>
@@ -1392,27 +1408,27 @@
       <c r="P15" t="s">
         <v>63</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>6</v>
       </c>
-      <c r="S15" s="1" t="str">
+      <c r="U15" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47GKd25","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>0.16</v>
       </c>
-      <c r="U15">
+      <c r="W15">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.96</v>
       </c>
-      <c r="V15">
+      <c r="X15">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>904.17600000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>21</v>
       </c>
@@ -1428,26 +1444,26 @@
       <c r="P16" t="s">
         <v>63</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>12</v>
       </c>
-      <c r="S16" s="1" t="str">
+      <c r="U16" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>0.8</v>
       </c>
-      <c r="U16">
+      <c r="W16">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>9.6000000000000014</v>
       </c>
-      <c r="V16">
+      <c r="X16">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>9041.760000000002</v>
       </c>
     </row>
-    <row r="17" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>23</v>
       </c>
@@ -1463,27 +1479,27 @@
       <c r="P17" t="s">
         <v>63</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
-      <c r="S17" s="2" t="str">
+      <c r="U17" s="2" t="str">
         <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T17">
+      <c r="V17">
         <v>0.1</v>
       </c>
-      <c r="U17">
+      <c r="W17">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="V17">
+      <c r="X17">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>282.55500000000006</v>
       </c>
     </row>
-    <row r="18" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>24</v>
       </c>
@@ -1499,27 +1515,27 @@
       <c r="P18" t="s">
         <v>63</v>
       </c>
-      <c r="R18">
+      <c r="T18">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
-      <c r="S18" s="1" t="str">
+      <c r="U18" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/4qpAEMl","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T18" s="4">
+      <c r="V18" s="4">
         <v>1.59</v>
       </c>
-      <c r="U18">
+      <c r="W18">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>4.7700000000000005</v>
       </c>
-      <c r="V18">
+      <c r="X18">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>4492.6245000000008</v>
       </c>
     </row>
-    <row r="19" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>25</v>
       </c>
@@ -1535,27 +1551,27 @@
       <c r="P19" t="s">
         <v>63</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
-      <c r="S19" s="1" t="str">
+      <c r="U19" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3Wle1em","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>0.34</v>
       </c>
-      <c r="U19">
+      <c r="W19">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.02</v>
       </c>
-      <c r="V19">
+      <c r="X19">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>960.68700000000001</v>
       </c>
     </row>
-    <row r="20" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>26</v>
       </c>
@@ -1571,27 +1587,27 @@
       <c r="P20" t="s">
         <v>63</v>
       </c>
-      <c r="R20">
+      <c r="T20">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="S20" s="1" t="str">
+      <c r="U20" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47oFwIR","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>0.6</v>
       </c>
-      <c r="U20">
+      <c r="W20">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.2</v>
       </c>
-      <c r="V20">
+      <c r="X20">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>1130.22</v>
       </c>
     </row>
-    <row r="21" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>27</v>
       </c>
@@ -1607,26 +1623,26 @@
       <c r="P21" t="s">
         <v>63</v>
       </c>
-      <c r="R21">
+      <c r="T21">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="U21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>0.18</v>
       </c>
-      <c r="U21">
+      <c r="W21">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.36</v>
       </c>
-      <c r="V21">
+      <c r="X21">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>339.06599999999997</v>
       </c>
     </row>
-    <row r="22" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>29</v>
       </c>
@@ -1642,27 +1658,27 @@
       <c r="P22" t="s">
         <v>63</v>
       </c>
-      <c r="R22">
+      <c r="T22">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>12</v>
       </c>
-      <c r="S22" s="1" t="str">
+      <c r="U22" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47bBWDf","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <v>0.15</v>
       </c>
-      <c r="U22">
+      <c r="W22">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.7999999999999998</v>
       </c>
-      <c r="V22">
+      <c r="X22">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>1695.33</v>
       </c>
     </row>
-    <row r="23" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>31</v>
       </c>
@@ -1678,27 +1694,27 @@
       <c r="P23" t="s">
         <v>63</v>
       </c>
-      <c r="R23">
+      <c r="T23">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="S23" s="1" t="str">
+      <c r="U23" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/48K3Qr8","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T23">
+      <c r="V23">
         <v>0.23</v>
       </c>
-      <c r="U23">
+      <c r="W23">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.23</v>
       </c>
-      <c r="V23">
+      <c r="X23">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>216.62550000000002</v>
       </c>
     </row>
-    <row r="24" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>32</v>
       </c>
@@ -1717,27 +1733,27 @@
       <c r="P24" t="s">
         <v>63</v>
       </c>
-      <c r="R24">
+      <c r="T24">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="S24" s="1" t="str">
+      <c r="U24" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47slRYu","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <v>0.41</v>
       </c>
-      <c r="U24">
+      <c r="W24">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.82</v>
       </c>
-      <c r="V24">
+      <c r="X24">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>772.31700000000001</v>
       </c>
     </row>
-    <row r="25" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:24" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>33</v>
       </c>
@@ -1753,22 +1769,22 @@
       <c r="P25" t="s">
         <v>63</v>
       </c>
-      <c r="R25">
+      <c r="T25">
         <v>5</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="U25" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="U25">
+      <c r="W25">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>5</v>
       </c>
-      <c r="V25">
+      <c r="X25">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>4709.25</v>
       </c>
     </row>
-    <row r="26" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:24" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
         <v>73</v>
       </c>
@@ -1778,22 +1794,22 @@
       <c r="P26" t="s">
         <v>63</v>
       </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-      <c r="S26" s="1" t="s">
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="U26">
+      <c r="W26">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1</v>
       </c>
-      <c r="V26">
+      <c r="X26">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>941.85</v>
       </c>
     </row>
-    <row r="27" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:24" x14ac:dyDescent="0.3">
       <c r="N27" t="s">
         <v>100</v>
       </c>
@@ -1803,22 +1819,22 @@
       <c r="P27" t="s">
         <v>63</v>
       </c>
-      <c r="R27">
-        <v>1</v>
-      </c>
-      <c r="S27" s="1" t="s">
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="U27">
+      <c r="W27">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1</v>
       </c>
-      <c r="V27">
+      <c r="X27">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>941.85</v>
       </c>
     </row>
-    <row r="28" spans="5:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:24" x14ac:dyDescent="0.3">
       <c r="N28" t="s">
         <v>33</v>
       </c>
@@ -1828,31 +1844,31 @@
       <c r="P28" t="s">
         <v>63</v>
       </c>
-      <c r="R28">
-        <v>1</v>
-      </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="U28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="T28">
+      <c r="V28">
         <v>0.32</v>
       </c>
-      <c r="U28">
+      <c r="W28">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.32</v>
       </c>
-      <c r="V28">
+      <c r="X28">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>301.392</v>
       </c>
     </row>
-    <row r="29" spans="5:22" x14ac:dyDescent="0.3">
-      <c r="R29" s="6"/>
-      <c r="V29" s="3"/>
+    <row r="29" spans="5:24" x14ac:dyDescent="0.3">
+      <c r="T29" s="6"/>
+      <c r="X29" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S21" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
+    <hyperlink ref="U21" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -1868,7 +1884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EDAD98-4A51-48B0-BAE4-039E551A8C8C}">
   <dimension ref="B2:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix(schematics): schematic +V and GND was changed WIP
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="406" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EE91FA-2241-4505-AC8B-938DC92868D4}"/>
+  <xr:revisionPtr revIDLastSave="419" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0983711A-9E16-47DC-B2DB-150195FD928D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
@@ -929,7 +929,7 @@
   <dimension ref="A2:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fix(components): schematics for components modification WIP
modification of the components cause a bug in all schematics WIP
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="419" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0983711A-9E16-47DC-B2DB-150195FD928D}"/>
+  <xr:revisionPtr revIDLastSave="469" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BA0EC29-1550-423C-B849-BEEE459931D0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Componentes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="129">
   <si>
     <t>power input</t>
   </si>
@@ -399,6 +399,63 @@
   </si>
   <si>
     <t>FP Corregido</t>
+  </si>
+  <si>
+    <t>SODFL1608X70N</t>
+  </si>
+  <si>
+    <t>Sch  Corregido</t>
+  </si>
+  <si>
+    <t>TSON8_2-3X1S_TOS-L</t>
+  </si>
+  <si>
+    <t>XT60PWM</t>
+  </si>
+  <si>
+    <t>CAPC2012X94N</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>CAPC0402X22N</t>
+  </si>
+  <si>
+    <t>CAPC2012X140N</t>
+  </si>
+  <si>
+    <t>NEW PCBLIbrary</t>
+  </si>
+  <si>
+    <t>CAPC1608X80N</t>
+  </si>
+  <si>
+    <t>CAPC1608X90N</t>
+  </si>
+  <si>
+    <t>CAPC1005X70N</t>
+  </si>
+  <si>
+    <t>INDPM104104X480N</t>
+  </si>
+  <si>
+    <t>RES_CSSH0805_.002OHM_STP</t>
+  </si>
+  <si>
+    <t>FP-AF0402-IPC_A</t>
+  </si>
+  <si>
+    <t>RESC1608X55N</t>
+  </si>
+  <si>
+    <t>LEDC1608X85N</t>
+  </si>
+  <si>
+    <t>GRT033</t>
+  </si>
+  <si>
+    <t>GRM033D70J224ME01D</t>
   </si>
 </sst>
 </file>
@@ -567,13 +624,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:X29" totalsRowCount="1">
-  <autoFilter ref="N5:X28" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:Z29" totalsRowCount="1">
+  <autoFilter ref="N5:Z28" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{2A8164C2-2FB7-4C23-97F1-2EB7091D5D63}" name="COMPONENTES"/>
     <tableColumn id="9" xr3:uid="{916D2FE0-85EB-46DA-9799-D85CA8D5156F}" name="Part Number"/>
     <tableColumn id="8" xr3:uid="{B1046C3A-A1F3-421E-9436-C5BB3C6B237A}" name="Altium"/>
     <tableColumn id="10" xr3:uid="{2CEA38F0-0C3D-417B-A37F-12BD902EBA47}" name="PCBlibrary"/>
+    <tableColumn id="13" xr3:uid="{2B03112D-768E-4B24-BA12-EF1CD9491DBB}" name="NEW PCBLIbrary"/>
+    <tableColumn id="12" xr3:uid="{66492975-40D9-428C-86A9-603CEEEB080E}" name="Sch  Corregido"/>
     <tableColumn id="11" xr3:uid="{F6CD5E74-C2A7-497A-977E-F83F137C4127}" name="FP Corregido"/>
     <tableColumn id="7" xr3:uid="{ADE89E6D-F7FC-45CE-A5CB-99276119FEF7}" name="D"/>
     <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="5" totalsRowDxfId="1">
@@ -595,8 +654,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}" name="Tabla3" displayName="Tabla3" ref="W2:X3" totalsRowShown="0">
-  <autoFilter ref="W2:X3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}" name="Tabla3" displayName="Tabla3" ref="Y2:Z3" totalsRowShown="0">
+  <autoFilter ref="Y2:Z3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6441C57D-BDB7-4FF4-9BC8-CECA7F77E429}" name="TOTAL(USD)">
       <calculatedColumnFormula>SUM(Tabla2[CantX$(USD)])</calculatedColumnFormula>
@@ -926,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
-  <dimension ref="A2:X29"/>
+  <dimension ref="A2:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,43 +1006,45 @@
     <col min="14" max="14" width="17.44140625" customWidth="1"/>
     <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5546875" customWidth="1"/>
-    <col min="19" max="19" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.88671875" customWidth="1"/>
-    <col min="22" max="22" width="20.109375" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15.21875" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" customWidth="1"/>
+    <col min="21" max="21" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.88671875" customWidth="1"/>
+    <col min="24" max="24" width="20.109375" customWidth="1"/>
+    <col min="25" max="25" width="13.5546875" customWidth="1"/>
+    <col min="26" max="26" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="W2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y2" t="s">
         <v>39</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <f>SUM(Tabla2[CantX$(USD)])</f>
         <v>36.869999999999997</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <f>ROUND(SUM(Tabla2[CantX$(CLP)]),0)</f>
         <v>34727</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1027,28 +1088,34 @@
         <v>108</v>
       </c>
       <c r="R5" t="s">
+        <v>118</v>
+      </c>
+      <c r="S5" t="s">
+        <v>111</v>
+      </c>
+      <c r="T5" t="s">
         <v>109</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>61</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>37</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" t="s">
         <v>38</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>41</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
         <v>42</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1067,27 +1134,30 @@
       <c r="P6" t="s">
         <v>63</v>
       </c>
-      <c r="T6">
+      <c r="Q6" t="s">
+        <v>110</v>
+      </c>
+      <c r="V6">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="U6" s="1" t="str">
+      <c r="W6" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/42XoOiu","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>0.34</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.34</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>320.22900000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1106,27 +1176,30 @@
       <c r="P7" t="s">
         <v>63</v>
       </c>
-      <c r="T7">
+      <c r="Q7" t="s">
+        <v>112</v>
+      </c>
+      <c r="V7">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="U7" s="1" t="str">
+      <c r="W7" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3Jxp5Cd","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>1.1100000000000001</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="X7">
+      <c r="Z7">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>1045.4535000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1148,27 +1221,33 @@
       <c r="P8" t="s">
         <v>63</v>
       </c>
-      <c r="T8">
+      <c r="Q8" t="s">
+        <v>113</v>
+      </c>
+      <c r="S8" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>4</v>
       </c>
-      <c r="U8" s="1" t="str">
+      <c r="W8" s="1" t="str">
         <f>HYPERLINK("https://octopart.com/es/xt60pw-m-amass-118051292","Octopart")</f>
         <v>Octopart</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>0.9</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>3.6</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],942)</f>
         <v>3391.2000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1187,26 +1266,29 @@
       <c r="P9" t="s">
         <v>63</v>
       </c>
-      <c r="T9">
+      <c r="Q9" t="s">
+        <v>114</v>
+      </c>
+      <c r="V9">
         <v>3</v>
       </c>
-      <c r="U9" s="1" t="str">
+      <c r="W9" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>0.1</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>282.55500000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1225,27 +1307,30 @@
       <c r="P10" t="s">
         <v>63</v>
       </c>
-      <c r="T10">
+      <c r="Q10" t="s">
+        <v>115</v>
+      </c>
+      <c r="V10">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="U10" s="1" t="str">
+      <c r="W10" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47aSprm","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>0.44</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.44</v>
       </c>
-      <c r="X10">
+      <c r="Z10">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>414.41399999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>17</v>
       </c>
@@ -1261,27 +1346,30 @@
       <c r="P11" t="s">
         <v>63</v>
       </c>
-      <c r="T11">
+      <c r="Q11" t="s">
+        <v>116</v>
+      </c>
+      <c r="V11">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="U11" s="2" t="str">
+      <c r="W11" s="2" t="str">
         <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>0.1</v>
       </c>
-      <c r="W11">
+      <c r="Y11">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.1</v>
       </c>
-      <c r="X11">
+      <c r="Z11">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>94.185000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>18</v>
       </c>
@@ -1300,27 +1388,30 @@
       <c r="P12" t="s">
         <v>63</v>
       </c>
-      <c r="T12">
+      <c r="Q12" t="s">
+        <v>117</v>
+      </c>
+      <c r="V12">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>4</v>
       </c>
-      <c r="U12" s="1" t="str">
+      <c r="W12" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/4oCNLrW","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V12">
+      <c r="X12">
         <v>0.42</v>
       </c>
-      <c r="W12">
+      <c r="Y12">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.68</v>
       </c>
-      <c r="X12">
+      <c r="Z12">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>1582.308</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>19</v>
       </c>
@@ -1336,27 +1427,30 @@
       <c r="P13" t="s">
         <v>63</v>
       </c>
-      <c r="T13">
+      <c r="Q13" t="s">
+        <v>119</v>
+      </c>
+      <c r="V13">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="U13" s="1" t="str">
+      <c r="W13" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/43ubkLk","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V13">
+      <c r="X13">
         <v>0.24</v>
       </c>
-      <c r="W13">
+      <c r="Y13">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.24</v>
       </c>
-      <c r="X13">
+      <c r="Z13">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>226.04400000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>22</v>
       </c>
@@ -1372,27 +1466,27 @@
       <c r="P14" t="s">
         <v>63</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="U14" s="1" t="str">
+      <c r="W14" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V14">
+      <c r="X14">
         <v>0.34</v>
       </c>
-      <c r="W14">
+      <c r="Y14">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.68</v>
       </c>
-      <c r="X14">
+      <c r="Z14">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>640.45800000000008</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>20</v>
       </c>
@@ -1408,27 +1502,30 @@
       <c r="P15" t="s">
         <v>63</v>
       </c>
-      <c r="T15">
+      <c r="Q15" t="s">
+        <v>120</v>
+      </c>
+      <c r="V15">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>6</v>
       </c>
-      <c r="U15" s="1" t="str">
+      <c r="W15" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47GKd25","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V15">
+      <c r="X15">
         <v>0.16</v>
       </c>
-      <c r="W15">
+      <c r="Y15">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.96</v>
       </c>
-      <c r="X15">
+      <c r="Z15">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>904.17600000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>21</v>
       </c>
@@ -1444,26 +1541,29 @@
       <c r="P16" t="s">
         <v>63</v>
       </c>
-      <c r="T16">
+      <c r="Q16" t="s">
+        <v>78</v>
+      </c>
+      <c r="V16">
         <v>12</v>
       </c>
-      <c r="U16" s="1" t="str">
+      <c r="W16" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V16">
+      <c r="X16">
         <v>0.8</v>
       </c>
-      <c r="W16">
+      <c r="Y16">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>9.6000000000000014</v>
       </c>
-      <c r="X16">
+      <c r="Z16">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>9041.760000000002</v>
       </c>
     </row>
-    <row r="17" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>23</v>
       </c>
@@ -1479,27 +1579,30 @@
       <c r="P17" t="s">
         <v>63</v>
       </c>
-      <c r="T17">
+      <c r="Q17" t="s">
+        <v>121</v>
+      </c>
+      <c r="V17">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
-      <c r="U17" s="2" t="str">
+      <c r="W17" s="2" t="str">
         <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V17">
+      <c r="X17">
         <v>0.1</v>
       </c>
-      <c r="W17">
+      <c r="Y17">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="X17">
+      <c r="Z17">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>282.55500000000006</v>
       </c>
     </row>
-    <row r="18" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>24</v>
       </c>
@@ -1515,27 +1618,30 @@
       <c r="P18" t="s">
         <v>63</v>
       </c>
-      <c r="T18">
+      <c r="Q18" t="s">
+        <v>122</v>
+      </c>
+      <c r="V18">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
-      <c r="U18" s="1" t="str">
+      <c r="W18" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/4qpAEMl","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V18" s="4">
+      <c r="X18" s="4">
         <v>1.59</v>
       </c>
-      <c r="W18">
+      <c r="Y18">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>4.7700000000000005</v>
       </c>
-      <c r="X18">
+      <c r="Z18">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>4492.6245000000008</v>
       </c>
     </row>
-    <row r="19" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>25</v>
       </c>
@@ -1551,27 +1657,30 @@
       <c r="P19" t="s">
         <v>63</v>
       </c>
-      <c r="T19">
+      <c r="Q19" t="s">
+        <v>97</v>
+      </c>
+      <c r="V19">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
-      <c r="U19" s="1" t="str">
+      <c r="W19" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3Wle1em","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V19">
+      <c r="X19">
         <v>0.34</v>
       </c>
-      <c r="W19">
+      <c r="Y19">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.02</v>
       </c>
-      <c r="X19">
+      <c r="Z19">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>960.68700000000001</v>
       </c>
     </row>
-    <row r="20" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>26</v>
       </c>
@@ -1587,27 +1696,30 @@
       <c r="P20" t="s">
         <v>63</v>
       </c>
-      <c r="T20">
+      <c r="Q20" t="s">
+        <v>123</v>
+      </c>
+      <c r="V20">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="U20" s="1" t="str">
+      <c r="W20" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47oFwIR","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V20">
+      <c r="X20">
         <v>0.6</v>
       </c>
-      <c r="W20">
+      <c r="Y20">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.2</v>
       </c>
-      <c r="X20">
+      <c r="Z20">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>1130.22</v>
       </c>
     </row>
-    <row r="21" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>27</v>
       </c>
@@ -1623,26 +1735,29 @@
       <c r="P21" t="s">
         <v>63</v>
       </c>
-      <c r="T21">
+      <c r="Q21" t="s">
+        <v>124</v>
+      </c>
+      <c r="V21">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="W21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="V21">
+      <c r="X21">
         <v>0.18</v>
       </c>
-      <c r="W21">
+      <c r="Y21">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.36</v>
       </c>
-      <c r="X21">
+      <c r="Z21">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>339.06599999999997</v>
       </c>
     </row>
-    <row r="22" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>29</v>
       </c>
@@ -1658,27 +1773,30 @@
       <c r="P22" t="s">
         <v>63</v>
       </c>
-      <c r="T22">
+      <c r="Q22" t="s">
+        <v>125</v>
+      </c>
+      <c r="V22">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>12</v>
       </c>
-      <c r="U22" s="1" t="str">
+      <c r="W22" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47bBWDf","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V22">
+      <c r="X22">
         <v>0.15</v>
       </c>
-      <c r="W22">
+      <c r="Y22">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1.7999999999999998</v>
       </c>
-      <c r="X22">
+      <c r="Z22">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>1695.33</v>
       </c>
     </row>
-    <row r="23" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>31</v>
       </c>
@@ -1694,27 +1812,30 @@
       <c r="P23" t="s">
         <v>63</v>
       </c>
-      <c r="T23">
+      <c r="Q23" t="s">
+        <v>125</v>
+      </c>
+      <c r="V23">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="U23" s="1" t="str">
+      <c r="W23" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/48K3Qr8","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V23">
+      <c r="X23">
         <v>0.23</v>
       </c>
-      <c r="W23">
+      <c r="Y23">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.23</v>
       </c>
-      <c r="X23">
+      <c r="Z23">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>216.62550000000002</v>
       </c>
     </row>
-    <row r="24" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>32</v>
       </c>
@@ -1733,27 +1854,30 @@
       <c r="P24" t="s">
         <v>63</v>
       </c>
-      <c r="T24">
+      <c r="Q24" t="s">
+        <v>126</v>
+      </c>
+      <c r="V24">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="U24" s="1" t="str">
+      <c r="W24" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47slRYu","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="V24">
+      <c r="X24">
         <v>0.41</v>
       </c>
-      <c r="W24">
+      <c r="Y24">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.82</v>
       </c>
-      <c r="X24">
+      <c r="Z24">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>772.31700000000001</v>
       </c>
     </row>
-    <row r="25" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>33</v>
       </c>
@@ -1769,22 +1893,25 @@
       <c r="P25" t="s">
         <v>63</v>
       </c>
-      <c r="T25">
+      <c r="Q25" t="s">
+        <v>127</v>
+      </c>
+      <c r="V25">
         <v>5</v>
       </c>
-      <c r="U25" s="1" t="s">
+      <c r="W25" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="W25">
+      <c r="Y25">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>5</v>
       </c>
-      <c r="X25">
+      <c r="Z25">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>4709.25</v>
       </c>
     </row>
-    <row r="26" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
         <v>73</v>
       </c>
@@ -1794,22 +1921,25 @@
       <c r="P26" t="s">
         <v>63</v>
       </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
-      <c r="U26" s="1" t="s">
+      <c r="Q26" t="s">
+        <v>120</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="W26">
+      <c r="Y26">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1</v>
       </c>
-      <c r="X26">
+      <c r="Z26">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>941.85</v>
       </c>
     </row>
-    <row r="27" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N27" t="s">
         <v>100</v>
       </c>
@@ -1819,22 +1949,25 @@
       <c r="P27" t="s">
         <v>63</v>
       </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
-      <c r="U27" s="1" t="s">
+      <c r="Q27" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="W27">
+      <c r="Y27">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>1</v>
       </c>
-      <c r="X27">
+      <c r="Z27">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>941.85</v>
       </c>
     </row>
-    <row r="28" spans="5:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N28" t="s">
         <v>33</v>
       </c>
@@ -1844,31 +1977,34 @@
       <c r="P28" t="s">
         <v>63</v>
       </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
-      <c r="U28" s="1" t="s">
+      <c r="Q28" t="s">
+        <v>125</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="V28">
+      <c r="X28">
         <v>0.32</v>
       </c>
-      <c r="W28">
+      <c r="Y28">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.32</v>
       </c>
-      <c r="X28">
+      <c r="Z28">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>301.392</v>
       </c>
     </row>
-    <row r="29" spans="5:24" x14ac:dyDescent="0.3">
-      <c r="T29" s="6"/>
-      <c r="X29" s="3"/>
+    <row r="29" spans="5:26" x14ac:dyDescent="0.3">
+      <c r="V29" s="6"/>
+      <c r="Z29" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U21" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
+    <hyperlink ref="W21" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
fix(footprint): some footprint was fixed WIP
fixed footprint component is registered in the excel
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="469" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BA0EC29-1550-423C-B849-BEEE459931D0}"/>
+  <xr:revisionPtr revIDLastSave="562" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8017FCFA-346F-42BF-9C16-7AC53DFEC719}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Componentes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="141">
   <si>
     <t>power input</t>
   </si>
@@ -456,6 +456,42 @@
   </si>
   <si>
     <t>GRM033D70J224ME01D</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>DIODO</t>
+  </si>
+  <si>
+    <t>CHIP</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>CAPACITOR</t>
+  </si>
+  <si>
+    <t>RESISTOR</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>RESC2013X06N</t>
+  </si>
+  <si>
+    <t>RESC1005X04N</t>
+  </si>
+  <si>
+    <t>CAPC2012X05N</t>
+  </si>
+  <si>
+    <t>X (so close)</t>
+  </si>
+  <si>
+    <t>CAPC1608X10N</t>
   </si>
 </sst>
 </file>
@@ -626,15 +662,18 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:Z29" totalsRowCount="1">
   <autoFilter ref="N5:Z28" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N6:Z28">
+    <sortCondition ref="O5:O28"/>
+  </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{2A8164C2-2FB7-4C23-97F1-2EB7091D5D63}" name="COMPONENTES"/>
+    <tableColumn id="7" xr3:uid="{1B66CD5D-E06C-4FE7-9C8A-156F9A991661}" name="Tipo"/>
     <tableColumn id="9" xr3:uid="{916D2FE0-85EB-46DA-9799-D85CA8D5156F}" name="Part Number"/>
     <tableColumn id="8" xr3:uid="{B1046C3A-A1F3-421E-9436-C5BB3C6B237A}" name="Altium"/>
     <tableColumn id="10" xr3:uid="{2CEA38F0-0C3D-417B-A37F-12BD902EBA47}" name="PCBlibrary"/>
     <tableColumn id="13" xr3:uid="{2B03112D-768E-4B24-BA12-EF1CD9491DBB}" name="NEW PCBLIbrary"/>
     <tableColumn id="12" xr3:uid="{66492975-40D9-428C-86A9-603CEEEB080E}" name="Sch  Corregido"/>
     <tableColumn id="11" xr3:uid="{F6CD5E74-C2A7-497A-977E-F83F137C4127}" name="FP Corregido"/>
-    <tableColumn id="7" xr3:uid="{ADE89E6D-F7FC-45CE-A5CB-99276119FEF7}" name="D"/>
     <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="5" totalsRowDxfId="1">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</calculatedColumnFormula>
     </tableColumn>
@@ -987,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
   <dimension ref="A2:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,14 +1042,13 @@
     <col min="11" max="11" width="16.109375" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="17.44140625" customWidth="1"/>
-    <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.6640625" customWidth="1"/>
-    <col min="19" max="19" width="15.21875" customWidth="1"/>
-    <col min="20" max="20" width="12.5546875" customWidth="1"/>
-    <col min="21" max="21" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.44140625" customWidth="1"/>
+    <col min="16" max="16" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.21875" customWidth="1"/>
+    <col min="21" max="21" width="12.5546875" customWidth="1"/>
     <col min="22" max="22" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.88671875" customWidth="1"/>
     <col min="24" max="24" width="20.109375" customWidth="1"/>
@@ -1030,13 +1068,13 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" t="e">
         <f>SUM(Tabla2[CantX$(USD)])</f>
-        <v>36.869999999999997</v>
-      </c>
-      <c r="Z3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z3" t="e">
         <f>ROUND(SUM(Tabla2[CantX$(CLP)]),0)</f>
-        <v>34727</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -1079,25 +1117,25 @@
         <v>13</v>
       </c>
       <c r="O5" t="s">
+        <v>129</v>
+      </c>
+      <c r="P5" t="s">
         <v>77</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>70</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>108</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>118</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>111</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>109</v>
-      </c>
-      <c r="U5" t="s">
-        <v>61</v>
       </c>
       <c r="V5" t="s">
         <v>37</v>
@@ -1126,35 +1164,46 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="P6" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="Q6" t="s">
-        <v>110</v>
+        <v>63</v>
+      </c>
+      <c r="R6" t="s">
+        <v>114</v>
+      </c>
+      <c r="S6" t="s">
+        <v>138</v>
+      </c>
+      <c r="T6" t="s">
+        <v>63</v>
+      </c>
+      <c r="U6" t="s">
+        <v>139</v>
       </c>
       <c r="V6">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W6" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/42XoOiu","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X6">
-        <v>0.34</v>
+        <v>0.1</v>
       </c>
       <c r="Y6">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.34</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="Z6">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>320.22900000000004</v>
+        <v>282.55500000000006</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -1168,35 +1217,47 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O7" t="s">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="P7" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="Q7" t="s">
-        <v>112</v>
+        <v>63</v>
+      </c>
+      <c r="R7" t="s">
+        <v>115</v>
+      </c>
+      <c r="S7" t="s">
+        <v>140</v>
+      </c>
+      <c r="T7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" t="s">
+        <v>63</v>
       </c>
       <c r="V7">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
       <c r="W7" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3Jxp5Cd","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47aSprm","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X7">
-        <v>1.1100000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="Y7">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.1100000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="Z7">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>1045.4535000000001</v>
+        <v>414.41399999999999</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -1213,38 +1274,44 @@
         <v>2</v>
       </c>
       <c r="N8" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="O8" t="s">
-        <v>14</v>
+        <v>133</v>
       </c>
       <c r="P8" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="Q8" t="s">
-        <v>113</v>
+        <v>63</v>
+      </c>
+      <c r="R8" t="s">
+        <v>116</v>
       </c>
       <c r="S8" t="s">
+        <v>116</v>
+      </c>
+      <c r="T8" t="s">
         <v>63</v>
       </c>
       <c r="V8">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>4</v>
       </c>
-      <c r="W8" s="1" t="str">
-        <f>HYPERLINK("https://octopart.com/es/xt60pw-m-amass-118051292","Octopart")</f>
-        <v>Octopart</v>
+      <c r="W8" s="2" t="str">
+        <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
+        <v>Mouser</v>
       </c>
       <c r="X8">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="Y8">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>3.6</v>
+        <v>0.4</v>
       </c>
       <c r="Z8">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],942)</f>
-        <v>3391.2000000000003</v>
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>376.74</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -1258,34 +1325,44 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="O9" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="P9" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="Q9" t="s">
-        <v>114</v>
+        <v>63</v>
+      </c>
+      <c r="R9" t="s">
+        <v>117</v>
+      </c>
+      <c r="S9" t="s">
+        <v>117</v>
+      </c>
+      <c r="T9" t="s">
+        <v>63</v>
       </c>
       <c r="V9">
-        <v>3</v>
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>1</v>
       </c>
       <c r="W9" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/4oCNLrW","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X9">
-        <v>0.1</v>
+        <v>0.42</v>
       </c>
       <c r="Y9">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.30000000000000004</v>
+        <v>0.42</v>
       </c>
       <c r="Z9">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>282.55500000000006</v>
+        <v>395.577</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
@@ -1299,35 +1376,44 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O10" t="s">
-        <v>82</v>
+        <v>133</v>
       </c>
       <c r="P10" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="Q10" t="s">
-        <v>115</v>
+        <v>63</v>
+      </c>
+      <c r="R10" t="s">
+        <v>119</v>
+      </c>
+      <c r="S10" t="s">
+        <v>119</v>
+      </c>
+      <c r="T10" t="s">
+        <v>63</v>
       </c>
       <c r="V10">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
       <c r="W10" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47aSprm","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/43ubkLk","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X10">
-        <v>0.44</v>
+        <v>0.24</v>
       </c>
       <c r="Y10">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.44</v>
+        <v>0.24</v>
       </c>
       <c r="Z10">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>414.41399999999999</v>
+        <v>226.04400000000001</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
@@ -1338,35 +1424,38 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="O11" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="P11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="Q11" t="s">
-        <v>116</v>
+        <v>63</v>
+      </c>
+      <c r="T11" t="s">
+        <v>63</v>
       </c>
       <c r="V11">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="W11" s="2" t="str">
-        <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
+      <c r="W11" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X11">
-        <v>0.1</v>
+        <v>0.34</v>
       </c>
       <c r="Y11">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.1</v>
+        <v>0.34</v>
       </c>
       <c r="Z11">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>94.185000000000002</v>
+        <v>320.22900000000004</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
@@ -1380,35 +1469,41 @@
         <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O12" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="P12" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="Q12" t="s">
-        <v>117</v>
+        <v>63</v>
+      </c>
+      <c r="R12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T12" t="s">
+        <v>63</v>
       </c>
       <c r="V12">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>4</v>
       </c>
       <c r="W12" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/4oCNLrW","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47GKd25","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X12">
-        <v>0.42</v>
+        <v>0.16</v>
       </c>
       <c r="Y12">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.68</v>
+        <v>0.64</v>
       </c>
       <c r="Z12">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>1582.308</v>
+        <v>602.78399999999999</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
@@ -1419,35 +1514,40 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="O13" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="P13" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="Q13" t="s">
-        <v>119</v>
+        <v>63</v>
+      </c>
+      <c r="R13" t="s">
+        <v>78</v>
+      </c>
+      <c r="T13" t="s">
+        <v>63</v>
       </c>
       <c r="V13">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="W13" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/43ubkLk","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X13">
-        <v>0.24</v>
+        <v>0.8</v>
       </c>
       <c r="Y13">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.24</v>
+        <v>9.6000000000000014</v>
       </c>
       <c r="Z13">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>226.04400000000001</v>
+        <v>9041.760000000002</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -1458,32 +1558,41 @@
         <v>2</v>
       </c>
       <c r="N14" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="O14" t="s">
-        <v>72</v>
+        <v>133</v>
       </c>
       <c r="P14" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>63</v>
+      </c>
+      <c r="R14" t="s">
+        <v>121</v>
+      </c>
+      <c r="T14" t="s">
         <v>63</v>
       </c>
       <c r="V14">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="W14" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
+      <c r="W14" s="2" t="str">
+        <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X14">
-        <v>0.34</v>
+        <v>0.1</v>
       </c>
       <c r="Y14">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.68</v>
+        <v>0.2</v>
       </c>
       <c r="Z14">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>640.45800000000008</v>
+        <v>188.37</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -1494,35 +1603,36 @@
         <v>6</v>
       </c>
       <c r="N15" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="O15" t="s">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="P15" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="Q15" t="s">
-        <v>120</v>
+        <v>63</v>
+      </c>
+      <c r="R15" t="s">
+        <v>127</v>
+      </c>
+      <c r="T15" t="s">
+        <v>63</v>
       </c>
       <c r="V15">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>6</v>
-      </c>
-      <c r="W15" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47GKd25","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X15">
-        <v>0.16</v>
+        <v>5</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Y15">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.96</v>
+        <v>5</v>
       </c>
       <c r="Z15">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>904.17600000000004</v>
+        <v>4709.25</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -1533,34 +1643,36 @@
         <v>3</v>
       </c>
       <c r="N16" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="O16" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="P16" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="Q16" t="s">
-        <v>78</v>
+        <v>63</v>
+      </c>
+      <c r="R16" t="s">
+        <v>120</v>
+      </c>
+      <c r="T16" t="s">
+        <v>63</v>
       </c>
       <c r="V16">
-        <v>12</v>
-      </c>
-      <c r="W16" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X16">
-        <v>0.8</v>
+        <v>1</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="Y16">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>9.6000000000000014</v>
+        <v>1</v>
       </c>
       <c r="Z16">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>9041.760000000002</v>
+        <v>941.85</v>
       </c>
     </row>
     <row r="17" spans="5:26" x14ac:dyDescent="0.3">
@@ -1571,35 +1683,36 @@
         <v>3</v>
       </c>
       <c r="N17" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="P17" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="Q17" t="s">
-        <v>121</v>
+        <v>63</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="T17" t="s">
+        <v>63</v>
       </c>
       <c r="V17">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>3</v>
-      </c>
-      <c r="W17" s="2" t="str">
-        <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X17">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="Y17">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.30000000000000004</v>
+        <v>1</v>
       </c>
       <c r="Z17">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>282.55500000000006</v>
+        <v>941.85</v>
       </c>
     </row>
     <row r="18" spans="5:26" x14ac:dyDescent="0.3">
@@ -1610,35 +1723,44 @@
         <v>3</v>
       </c>
       <c r="N18" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="O18" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="P18" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="Q18" t="s">
-        <v>122</v>
+        <v>63</v>
+      </c>
+      <c r="R18" t="s">
+        <v>112</v>
+      </c>
+      <c r="T18" t="s">
+        <v>63</v>
+      </c>
+      <c r="U18" t="s">
+        <v>63</v>
       </c>
       <c r="V18">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
       <c r="W18" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/4qpAEMl","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/3Jxp5Cd","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="X18" s="4">
-        <v>1.59</v>
+      <c r="X18">
+        <v>1.1100000000000001</v>
       </c>
       <c r="Y18">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>4.7700000000000005</v>
+        <v>3.33</v>
       </c>
       <c r="Z18">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>4492.6245000000008</v>
+        <v>3136.3605000000002</v>
       </c>
     </row>
     <row r="19" spans="5:26" x14ac:dyDescent="0.3">
@@ -1649,35 +1771,44 @@
         <v>3</v>
       </c>
       <c r="N19" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="O19" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="P19" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="Q19" t="s">
-        <v>97</v>
+        <v>63</v>
+      </c>
+      <c r="R19" t="s">
+        <v>113</v>
+      </c>
+      <c r="T19" t="s">
+        <v>63</v>
+      </c>
+      <c r="U19" t="s">
+        <v>63</v>
       </c>
       <c r="V19">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
       <c r="W19" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3Wle1em","Mouser")</f>
-        <v>Mouser</v>
+        <f>HYPERLINK("https://octopart.com/es/xt60pw-m-amass-118051292","Octopart")</f>
+        <v>Octopart</v>
       </c>
       <c r="X19">
-        <v>0.34</v>
+        <v>0.9</v>
       </c>
       <c r="Y19">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.02</v>
+        <v>2.7</v>
       </c>
       <c r="Z19">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>960.68700000000001</v>
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],942)</f>
+        <v>2543.4</v>
       </c>
     </row>
     <row r="20" spans="5:26" x14ac:dyDescent="0.3">
@@ -1688,35 +1819,41 @@
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O20" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="P20" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="Q20" t="s">
-        <v>123</v>
+        <v>63</v>
+      </c>
+      <c r="R20" t="s">
+        <v>110</v>
+      </c>
+      <c r="T20" t="s">
+        <v>63</v>
       </c>
       <c r="V20">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
       <c r="W20" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47oFwIR","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/42XoOiu","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X20">
-        <v>0.6</v>
+        <v>0.34</v>
       </c>
       <c r="Y20">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.2</v>
+        <v>0.68</v>
       </c>
       <c r="Z20">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>1130.22</v>
+        <v>640.45800000000008</v>
       </c>
     </row>
     <row r="21" spans="5:26" x14ac:dyDescent="0.3">
@@ -1727,34 +1864,41 @@
         <v>2</v>
       </c>
       <c r="N21" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="O21" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="P21" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="Q21" t="s">
-        <v>124</v>
+        <v>63</v>
+      </c>
+      <c r="R21" t="s">
+        <v>97</v>
+      </c>
+      <c r="T21" t="s">
+        <v>63</v>
       </c>
       <c r="V21">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="W21" s="2" t="s">
-        <v>81</v>
+      <c r="W21" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/3Wle1em","Mouser")</f>
+        <v>Mouser</v>
       </c>
       <c r="X21">
-        <v>0.18</v>
+        <v>0.34</v>
       </c>
       <c r="Y21">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.36</v>
+        <v>0.68</v>
       </c>
       <c r="Z21">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>339.06599999999997</v>
+        <v>640.45800000000008</v>
       </c>
     </row>
     <row r="22" spans="5:26" x14ac:dyDescent="0.3">
@@ -1765,35 +1909,41 @@
         <v>12</v>
       </c>
       <c r="N22" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="O22" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="P22" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="Q22" t="s">
-        <v>125</v>
+        <v>63</v>
+      </c>
+      <c r="R22" t="s">
+        <v>126</v>
+      </c>
+      <c r="T22" t="s">
+        <v>63</v>
       </c>
       <c r="V22">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>12</v>
       </c>
       <c r="W22" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47bBWDf","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47slRYu","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X22">
-        <v>0.15</v>
+        <v>0.41</v>
       </c>
       <c r="Y22">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.7999999999999998</v>
+        <v>4.92</v>
       </c>
       <c r="Z22">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>1695.33</v>
+        <v>4633.902</v>
       </c>
     </row>
     <row r="23" spans="5:26" x14ac:dyDescent="0.3">
@@ -1804,35 +1954,41 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="O23" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="P23" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="Q23" t="s">
-        <v>125</v>
+        <v>63</v>
+      </c>
+      <c r="R23" t="s">
+        <v>122</v>
+      </c>
+      <c r="T23" t="s">
+        <v>63</v>
       </c>
       <c r="V23">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
       <c r="W23" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/48K3Qr8","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/4qpAEMl","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="X23">
-        <v>0.23</v>
+      <c r="X23" s="4">
+        <v>1.59</v>
       </c>
       <c r="Y23">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.23</v>
+        <v>1.59</v>
       </c>
       <c r="Z23">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>216.62550000000002</v>
+        <v>1497.5415</v>
       </c>
     </row>
     <row r="24" spans="5:26" x14ac:dyDescent="0.3">
@@ -1846,35 +2002,47 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="O24" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="P24" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q24" t="s">
-        <v>126</v>
+        <v>63</v>
+      </c>
+      <c r="R24" t="s">
+        <v>123</v>
+      </c>
+      <c r="S24" t="s">
+        <v>136</v>
+      </c>
+      <c r="T24" t="s">
+        <v>63</v>
+      </c>
+      <c r="U24" t="s">
+        <v>63</v>
       </c>
       <c r="V24">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
       <c r="W24" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47slRYu","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47oFwIR","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X24">
-        <v>0.41</v>
+        <v>0.6</v>
       </c>
       <c r="Y24">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.82</v>
+        <v>1.2</v>
       </c>
       <c r="Z24">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>772.31700000000001</v>
+        <v>1130.22</v>
       </c>
     </row>
     <row r="25" spans="5:26" x14ac:dyDescent="0.3">
@@ -1885,100 +2053,153 @@
         <v>2</v>
       </c>
       <c r="N25" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="O25" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="P25" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="Q25" t="s">
-        <v>127</v>
+        <v>63</v>
+      </c>
+      <c r="R25" t="s">
+        <v>124</v>
+      </c>
+      <c r="S25" t="s">
+        <v>137</v>
+      </c>
+      <c r="T25" t="s">
+        <v>63</v>
+      </c>
+      <c r="U25" t="s">
+        <v>63</v>
       </c>
       <c r="V25">
-        <v>5</v>
-      </c>
-      <c r="W25" s="1" t="s">
-        <v>105</v>
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>2</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="X25">
+        <v>0.18</v>
       </c>
       <c r="Y25">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>5</v>
+        <v>0.36</v>
       </c>
       <c r="Z25">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>4709.25</v>
+        <v>339.06599999999997</v>
       </c>
     </row>
     <row r="26" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="O26" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="P26" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="Q26" t="s">
-        <v>120</v>
-      </c>
-      <c r="V26">
-        <v>1</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y26">
+        <v>63</v>
+      </c>
+      <c r="R26" t="s">
+        <v>125</v>
+      </c>
+      <c r="S26" t="s">
+        <v>125</v>
+      </c>
+      <c r="T26" t="s">
+        <v>63</v>
+      </c>
+      <c r="V26" t="e">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W26" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/47bBWDf","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="X26">
+        <v>0.15</v>
+      </c>
+      <c r="Y26" t="e">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1</v>
-      </c>
-      <c r="Z26">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z26" t="e">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>941.85</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N27" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="O27" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="P27" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q27" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="V27">
-        <v>1</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y27">
+        <v>89</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>63</v>
+      </c>
+      <c r="R27" t="s">
+        <v>125</v>
+      </c>
+      <c r="S27" t="s">
+        <v>125</v>
+      </c>
+      <c r="T27" t="s">
+        <v>63</v>
+      </c>
+      <c r="V27" t="e">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W27" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/48K3Qr8","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="X27">
+        <v>0.23</v>
+      </c>
+      <c r="Y27" t="e">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1</v>
-      </c>
-      <c r="Z27">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z27" t="e">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>941.85</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N28" t="s">
         <v>33</v>
       </c>
-      <c r="O28" s="4" t="s">
+      <c r="O28" t="s">
+        <v>134</v>
+      </c>
+      <c r="P28" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P28" t="s">
-        <v>63</v>
-      </c>
       <c r="Q28" t="s">
+        <v>63</v>
+      </c>
+      <c r="R28" t="s">
         <v>125</v>
+      </c>
+      <c r="S28" t="s">
+        <v>125</v>
+      </c>
+      <c r="T28" t="s">
+        <v>63</v>
       </c>
       <c r="V28">
         <v>1</v>
@@ -2004,7 +2225,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W21" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
+    <hyperlink ref="W25" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
fix(footprint): All resistors and capacitor were fixed
resistors and capacitors were fixed by hand.
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="562" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8017FCFA-346F-42BF-9C16-7AC53DFEC719}"/>
+  <xr:revisionPtr revIDLastSave="605" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22D70B8D-870A-457A-BA75-C20FD29ADDE3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Componentes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="149">
   <si>
     <t>power input</t>
   </si>
@@ -492,6 +492,30 @@
   </si>
   <si>
     <t>CAPC1608X10N</t>
+  </si>
+  <si>
+    <t>CAPC0402X02L</t>
+  </si>
+  <si>
+    <t>CAPC2012X14N</t>
+  </si>
+  <si>
+    <t>CAPC1608X09N</t>
+  </si>
+  <si>
+    <t>CAPC3216X19N</t>
+  </si>
+  <si>
+    <t>CAPC1005X07N</t>
+  </si>
+  <si>
+    <t>CAPC0603X03N</t>
+  </si>
+  <si>
+    <t>CAPC0603X06N</t>
+  </si>
+  <si>
+    <t>RESC1608X06N</t>
   </si>
 </sst>
 </file>
@@ -663,7 +687,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:Z29" totalsRowCount="1">
   <autoFilter ref="N5:Z28" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N6:Z28">
-    <sortCondition ref="O5:O28"/>
+    <sortCondition ref="S5:S28"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{2A8164C2-2FB7-4C23-97F1-2EB7091D5D63}" name="COMPONENTES"/>
@@ -1026,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
   <dimension ref="A2:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,34 +1188,35 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="O6" t="s">
         <v>133</v>
       </c>
       <c r="P6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="Q6" t="s">
         <v>63</v>
       </c>
       <c r="R6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="S6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="T6" t="s">
         <v>63</v>
       </c>
       <c r="U6" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="V6">
-        <v>3</v>
-      </c>
-      <c r="W6" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>1</v>
+      </c>
+      <c r="W6" s="2" t="str">
+        <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X6">
@@ -1199,11 +1224,11 @@
       </c>
       <c r="Y6">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.30000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="Z6">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>282.55500000000006</v>
+        <v>94.185000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -1217,22 +1242,22 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="O7" t="s">
         <v>133</v>
       </c>
       <c r="P7" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="Q7" t="s">
         <v>63</v>
       </c>
       <c r="R7" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="S7" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="T7" t="s">
         <v>63</v>
@@ -1241,23 +1266,18 @@
         <v>63</v>
       </c>
       <c r="V7">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>1</v>
-      </c>
-      <c r="W7" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47aSprm","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X7">
-        <v>0.44</v>
+        <v>5</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Y7">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.44</v>
+        <v>5</v>
       </c>
       <c r="Z7">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>414.41399999999999</v>
+        <v>4709.25</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -1274,44 +1294,42 @@
         <v>2</v>
       </c>
       <c r="N8" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
         <v>133</v>
       </c>
       <c r="P8" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="Q8" t="s">
         <v>63</v>
       </c>
-      <c r="R8" t="s">
-        <v>116</v>
+      <c r="R8" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="S8" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="T8" t="s">
         <v>63</v>
       </c>
+      <c r="U8" t="s">
+        <v>63</v>
+      </c>
       <c r="V8">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>4</v>
-      </c>
-      <c r="W8" s="2" t="str">
-        <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X8">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="Y8">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>376.74</v>
+        <v>941.85</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -1325,44 +1343,47 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="O9" t="s">
         <v>133</v>
       </c>
       <c r="P9" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="Q9" t="s">
         <v>63</v>
       </c>
       <c r="R9" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="S9" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="T9" t="s">
+        <v>63</v>
+      </c>
+      <c r="U9" t="s">
         <v>63</v>
       </c>
       <c r="V9">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>1</v>
       </c>
-      <c r="W9" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/4oCNLrW","Mouser")</f>
+      <c r="W9" s="2" t="str">
+        <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X9">
-        <v>0.42</v>
+        <v>0.1</v>
       </c>
       <c r="Y9">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.42</v>
+        <v>0.1</v>
       </c>
       <c r="Z9">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>395.577</v>
+        <v>94.185000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
@@ -1391,9 +1412,12 @@
         <v>119</v>
       </c>
       <c r="S10" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="T10" t="s">
+        <v>63</v>
+      </c>
+      <c r="U10" t="s">
         <v>63</v>
       </c>
       <c r="V10">
@@ -1424,18 +1448,27 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="O11" t="s">
         <v>133</v>
       </c>
       <c r="P11" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="Q11" t="s">
         <v>63</v>
       </c>
+      <c r="R11" t="s">
+        <v>120</v>
+      </c>
+      <c r="S11" t="s">
+        <v>143</v>
+      </c>
       <c r="T11" t="s">
+        <v>63</v>
+      </c>
+      <c r="U11" t="s">
         <v>63</v>
       </c>
       <c r="V11">
@@ -1443,19 +1476,19 @@
         <v>1</v>
       </c>
       <c r="W11" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47GKd25","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X11">
-        <v>0.34</v>
+        <v>0.16</v>
       </c>
       <c r="Y11">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.34</v>
+        <v>0.16</v>
       </c>
       <c r="Z11">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>320.22900000000004</v>
+        <v>150.696</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
@@ -1469,13 +1502,13 @@
         <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="O12" t="s">
         <v>133</v>
       </c>
       <c r="P12" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="Q12" t="s">
         <v>63</v>
@@ -1483,27 +1516,28 @@
       <c r="R12" t="s">
         <v>120</v>
       </c>
+      <c r="S12" t="s">
+        <v>143</v>
+      </c>
       <c r="T12" t="s">
         <v>63</v>
       </c>
+      <c r="U12" t="s">
+        <v>63</v>
+      </c>
       <c r="V12">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>4</v>
-      </c>
-      <c r="W12" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47GKd25","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X12">
-        <v>0.16</v>
+        <v>1</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="Y12">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.64</v>
+        <v>1</v>
       </c>
       <c r="Z12">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>602.78399999999999</v>
+        <v>941.85</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
@@ -1514,40 +1548,47 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="O13" t="s">
         <v>133</v>
       </c>
       <c r="P13" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="Q13" t="s">
         <v>63</v>
       </c>
       <c r="R13" t="s">
-        <v>78</v>
+        <v>115</v>
+      </c>
+      <c r="S13" t="s">
+        <v>140</v>
       </c>
       <c r="T13" t="s">
         <v>63</v>
       </c>
+      <c r="U13" t="s">
+        <v>63</v>
+      </c>
       <c r="V13">
-        <v>12</v>
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>1</v>
       </c>
       <c r="W13" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47aSprm","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X13">
-        <v>0.8</v>
+        <v>0.44</v>
       </c>
       <c r="Y13">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>9.6000000000000014</v>
+        <v>0.44</v>
       </c>
       <c r="Z13">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>9041.760000000002</v>
+        <v>414.41399999999999</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -1558,29 +1599,34 @@
         <v>2</v>
       </c>
       <c r="N14" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="O14" t="s">
         <v>133</v>
       </c>
       <c r="P14" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="Q14" t="s">
         <v>63</v>
       </c>
       <c r="R14" t="s">
-        <v>121</v>
+        <v>114</v>
+      </c>
+      <c r="S14" t="s">
+        <v>138</v>
       </c>
       <c r="T14" t="s">
         <v>63</v>
       </c>
+      <c r="U14" t="s">
+        <v>139</v>
+      </c>
       <c r="V14">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>2</v>
-      </c>
-      <c r="W14" s="2" t="str">
-        <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
+        <v>3</v>
+      </c>
+      <c r="W14" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X14">
@@ -1588,11 +1634,11 @@
       </c>
       <c r="Y14">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="Z14">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>188.37</v>
+        <v>282.55500000000006</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -1603,36 +1649,44 @@
         <v>6</v>
       </c>
       <c r="N15" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="O15" t="s">
         <v>133</v>
       </c>
       <c r="P15" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="Q15" t="s">
         <v>63</v>
       </c>
-      <c r="R15" t="s">
-        <v>127</v>
+      <c r="S15" t="s">
+        <v>138</v>
       </c>
       <c r="T15" t="s">
         <v>63</v>
       </c>
+      <c r="U15" t="s">
+        <v>63</v>
+      </c>
       <c r="V15">
-        <v>5</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>105</v>
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>6</v>
+      </c>
+      <c r="W15" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="X15">
+        <v>0.34</v>
       </c>
       <c r="Y15">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>5</v>
+        <v>2.04</v>
       </c>
       <c r="Z15">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>4709.25</v>
+        <v>1921.374</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -1643,36 +1697,47 @@
         <v>3</v>
       </c>
       <c r="N16" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="O16" t="s">
         <v>133</v>
       </c>
       <c r="P16" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="Q16" t="s">
         <v>63</v>
       </c>
       <c r="R16" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="S16" t="s">
+        <v>142</v>
       </c>
       <c r="T16" t="s">
         <v>63</v>
       </c>
+      <c r="U16" t="s">
+        <v>63</v>
+      </c>
       <c r="V16">
-        <v>1</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>106</v>
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>3</v>
+      </c>
+      <c r="W16" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/4oCNLrW","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="X16">
+        <v>0.42</v>
       </c>
       <c r="Y16">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1</v>
+        <v>1.26</v>
       </c>
       <c r="Z16">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>941.85</v>
+        <v>1186.731</v>
       </c>
     </row>
     <row r="17" spans="5:26" x14ac:dyDescent="0.3">
@@ -1683,36 +1748,46 @@
         <v>3</v>
       </c>
       <c r="N17" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="O17" t="s">
         <v>133</v>
       </c>
       <c r="P17" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="Q17" t="s">
         <v>63</v>
       </c>
-      <c r="R17" s="6" t="s">
-        <v>128</v>
+      <c r="R17" t="s">
+        <v>78</v>
+      </c>
+      <c r="S17" t="s">
+        <v>144</v>
       </c>
       <c r="T17" t="s">
         <v>63</v>
       </c>
+      <c r="U17" t="s">
+        <v>63</v>
+      </c>
       <c r="V17">
-        <v>1</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>107</v>
+        <v>12</v>
+      </c>
+      <c r="W17" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="X17">
+        <v>0.8</v>
       </c>
       <c r="Y17">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1</v>
+        <v>9.6000000000000014</v>
       </c>
       <c r="Z17">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>941.85</v>
+        <v>9041.760000000002</v>
       </c>
     </row>
     <row r="18" spans="5:26" x14ac:dyDescent="0.3">
@@ -1723,19 +1798,22 @@
         <v>3</v>
       </c>
       <c r="N18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O18" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="P18" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q18" t="s">
         <v>63</v>
       </c>
       <c r="R18" t="s">
-        <v>112</v>
+        <v>124</v>
+      </c>
+      <c r="S18" t="s">
+        <v>137</v>
       </c>
       <c r="T18" t="s">
         <v>63</v>
@@ -1747,20 +1825,19 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>3</v>
       </c>
-      <c r="W18" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3Jxp5Cd","Mouser")</f>
-        <v>Mouser</v>
+      <c r="W18" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="X18">
-        <v>1.1100000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="Y18">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>3.33</v>
+        <v>0.54</v>
       </c>
       <c r="Z18">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>3136.3605000000002</v>
+        <v>508.59900000000005</v>
       </c>
     </row>
     <row r="19" spans="5:26" x14ac:dyDescent="0.3">
@@ -1771,19 +1848,22 @@
         <v>3</v>
       </c>
       <c r="N19" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="O19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="P19" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="Q19" t="s">
         <v>63</v>
       </c>
       <c r="R19" t="s">
-        <v>113</v>
+        <v>125</v>
+      </c>
+      <c r="S19" t="s">
+        <v>148</v>
       </c>
       <c r="T19" t="s">
         <v>63</v>
@@ -1796,19 +1876,19 @@
         <v>3</v>
       </c>
       <c r="W19" s="1" t="str">
-        <f>HYPERLINK("https://octopart.com/es/xt60pw-m-amass-118051292","Octopart")</f>
-        <v>Octopart</v>
+        <f>HYPERLINK("https://mou.sr/47bBWDf","Mouser")</f>
+        <v>Mouser</v>
       </c>
       <c r="X19">
-        <v>0.9</v>
+        <v>0.15</v>
       </c>
       <c r="Y19">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>2.7</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="Z19">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],942)</f>
-        <v>2543.4</v>
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>423.83249999999998</v>
       </c>
     </row>
     <row r="20" spans="5:26" x14ac:dyDescent="0.3">
@@ -1819,21 +1899,27 @@
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O20" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P20" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="Q20" t="s">
         <v>63</v>
       </c>
       <c r="R20" t="s">
-        <v>110</v>
+        <v>125</v>
+      </c>
+      <c r="S20" t="s">
+        <v>148</v>
       </c>
       <c r="T20" t="s">
+        <v>63</v>
+      </c>
+      <c r="U20" t="s">
         <v>63</v>
       </c>
       <c r="V20">
@@ -1841,19 +1927,19 @@
         <v>2</v>
       </c>
       <c r="W20" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/42XoOiu","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/48K3Qr8","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X20">
-        <v>0.34</v>
+        <v>0.23</v>
       </c>
       <c r="Y20">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.68</v>
+        <v>0.46</v>
       </c>
       <c r="Z20">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>640.45800000000008</v>
+        <v>433.25100000000003</v>
       </c>
     </row>
     <row r="21" spans="5:26" x14ac:dyDescent="0.3">
@@ -1864,41 +1950,45 @@
         <v>2</v>
       </c>
       <c r="N21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O21" t="s">
-        <v>130</v>
-      </c>
-      <c r="P21" t="s">
-        <v>97</v>
+        <v>134</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="Q21" t="s">
         <v>63</v>
       </c>
       <c r="R21" t="s">
-        <v>97</v>
+        <v>125</v>
+      </c>
+      <c r="S21" t="s">
+        <v>148</v>
       </c>
       <c r="T21" t="s">
         <v>63</v>
       </c>
+      <c r="U21" t="s">
+        <v>63</v>
+      </c>
       <c r="V21">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>2</v>
-      </c>
-      <c r="W21" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3Wle1em","Mouser")</f>
-        <v>Mouser</v>
+        <v>1</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="X21">
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
       <c r="Y21">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.68</v>
+        <v>0.32</v>
       </c>
       <c r="Z21">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>640.45800000000008</v>
+        <v>301.392</v>
       </c>
     </row>
     <row r="22" spans="5:26" x14ac:dyDescent="0.3">
@@ -1909,21 +1999,27 @@
         <v>12</v>
       </c>
       <c r="N22" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="O22" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P22" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="Q22" t="s">
         <v>63</v>
       </c>
       <c r="R22" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="S22" t="s">
+        <v>136</v>
       </c>
       <c r="T22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U22" t="s">
         <v>63</v>
       </c>
       <c r="V22">
@@ -1931,19 +2027,19 @@
         <v>12</v>
       </c>
       <c r="W22" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47slRYu","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47oFwIR","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X22">
-        <v>0.41</v>
+        <v>0.6</v>
       </c>
       <c r="Y22">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>4.92</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="Z22">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>4633.902</v>
+        <v>6781.32</v>
       </c>
     </row>
     <row r="23" spans="5:26" x14ac:dyDescent="0.3">
@@ -1954,21 +2050,24 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="O23" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="P23" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="Q23" t="s">
         <v>63</v>
       </c>
       <c r="R23" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="T23" t="s">
+        <v>63</v>
+      </c>
+      <c r="U23" t="s">
         <v>63</v>
       </c>
       <c r="V23">
@@ -1976,19 +2075,19 @@
         <v>1</v>
       </c>
       <c r="W23" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/4qpAEMl","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/3Jxp5Cd","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="X23" s="4">
-        <v>1.59</v>
+      <c r="X23">
+        <v>1.1100000000000001</v>
       </c>
       <c r="Y23">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.59</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="Z23">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>1497.5415</v>
+        <v>1045.4535000000001</v>
       </c>
     </row>
     <row r="24" spans="5:26" x14ac:dyDescent="0.3">
@@ -2002,22 +2101,19 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P24" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="Q24" t="s">
         <v>63</v>
       </c>
       <c r="R24" t="s">
-        <v>123</v>
-      </c>
-      <c r="S24" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="T24" t="s">
         <v>63</v>
@@ -2030,19 +2126,19 @@
         <v>2</v>
       </c>
       <c r="W24" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47oFwIR","Mouser")</f>
-        <v>Mouser</v>
+        <f>HYPERLINK("https://octopart.com/es/xt60pw-m-amass-118051292","Octopart")</f>
+        <v>Octopart</v>
       </c>
       <c r="X24">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="Y24">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="Z24">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>1130.22</v>
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],942)</f>
+        <v>1695.6000000000001</v>
       </c>
     </row>
     <row r="25" spans="5:26" x14ac:dyDescent="0.3">
@@ -2053,66 +2149,58 @@
         <v>2</v>
       </c>
       <c r="N25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="P25" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="Q25" t="s">
         <v>63</v>
       </c>
       <c r="R25" t="s">
-        <v>124</v>
-      </c>
-      <c r="S25" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="T25" t="s">
-        <v>63</v>
-      </c>
-      <c r="U25" t="s">
         <v>63</v>
       </c>
       <c r="V25">
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="W25" s="2" t="s">
-        <v>81</v>
+      <c r="W25" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/42XoOiu","Mouser")</f>
+        <v>Mouser</v>
       </c>
       <c r="X25">
-        <v>0.18</v>
+        <v>0.34</v>
       </c>
       <c r="Y25">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.36</v>
+        <v>0.68</v>
       </c>
       <c r="Z25">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>339.06599999999997</v>
+        <v>640.45800000000008</v>
       </c>
     </row>
     <row r="26" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="O26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="P26" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="Q26" t="s">
         <v>63</v>
       </c>
       <c r="R26" t="s">
-        <v>125</v>
-      </c>
-      <c r="S26" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="T26" t="s">
         <v>63</v>
@@ -2122,11 +2210,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="W26" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47bBWDf","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/3Wle1em","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X26">
-        <v>0.15</v>
+        <v>0.34</v>
       </c>
       <c r="Y26" t="e">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
@@ -2139,22 +2227,19 @@
     </row>
     <row r="27" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N27" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="O27" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="P27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q27" t="s">
         <v>63</v>
       </c>
       <c r="R27" t="s">
-        <v>125</v>
-      </c>
-      <c r="S27" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T27" t="s">
         <v>63</v>
@@ -2164,11 +2249,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="W27" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/48K3Qr8","Mouser")</f>
+        <f>HYPERLINK("https://mou.sr/47slRYu","Mouser")</f>
         <v>Mouser</v>
       </c>
       <c r="X27">
-        <v>0.23</v>
+        <v>0.41</v>
       </c>
       <c r="Y27" t="e">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
@@ -2181,42 +2266,41 @@
     </row>
     <row r="28" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N28" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="O28" t="s">
-        <v>134</v>
-      </c>
-      <c r="P28" s="4" t="s">
-        <v>91</v>
+        <v>135</v>
+      </c>
+      <c r="P28" t="s">
+        <v>93</v>
       </c>
       <c r="Q28" t="s">
         <v>63</v>
       </c>
       <c r="R28" t="s">
-        <v>125</v>
-      </c>
-      <c r="S28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="T28" t="s">
         <v>63</v>
       </c>
-      <c r="V28">
-        <v>1</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="X28">
-        <v>0.32</v>
-      </c>
-      <c r="Y28">
+      <c r="V28" t="e">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W28" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/4qpAEMl","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="X28" s="4">
+        <v>1.59</v>
+      </c>
+      <c r="Y28" t="e">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.32</v>
-      </c>
-      <c r="Z28">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z28" t="e">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>301.392</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="5:26" x14ac:dyDescent="0.3">
@@ -2225,14 +2309,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W25" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
+    <hyperlink ref="W18" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
+    <hyperlink ref="W7" r:id="rId2" xr:uid="{B765BA37-3C00-40F5-AEDD-838B98A4DF8E}"/>
+    <hyperlink ref="W12" r:id="rId3" xr:uid="{B0DD47A4-DB96-49FA-9651-714D11187895}"/>
+    <hyperlink ref="W8" r:id="rId4" xr:uid="{23FAA789-D6A4-48F6-B5EA-A3B0AFCD0314}"/>
+    <hyperlink ref="W21" r:id="rId5" xr:uid="{3AFEECC7-F076-4F50-A9F6-AB0039D9AEF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
   <tableParts count="3">
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix(footprint): all footprint passive components were fixed
All resistors, capacitors, inductors and diodos were fixed by hand
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="605" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22D70B8D-870A-457A-BA75-C20FD29ADDE3}"/>
+  <xr:revisionPtr revIDLastSave="620" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{867E0BD8-9CDD-4955-AF7F-3EBDB59F917B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="151">
   <si>
     <t>power input</t>
   </si>
@@ -488,9 +488,6 @@
     <t>CAPC2012X05N</t>
   </si>
   <si>
-    <t>X (so close)</t>
-  </si>
-  <si>
     <t>CAPC1608X10N</t>
   </si>
   <si>
@@ -516,6 +513,15 @@
   </si>
   <si>
     <t>RESC1608X06N</t>
+  </si>
+  <si>
+    <t>CONN_XT60PWM</t>
+  </si>
+  <si>
+    <t>XT60PW-M</t>
+  </si>
+  <si>
+    <t>DIOM4336X24N</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1076,7 @@
     <col min="16" max="16" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.6640625" customWidth="1"/>
+    <col min="19" max="19" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.21875" customWidth="1"/>
     <col min="21" max="21" width="12.5546875" customWidth="1"/>
     <col min="22" max="22" width="11.21875" bestFit="1" customWidth="1"/>
@@ -1203,7 +1209,7 @@
         <v>116</v>
       </c>
       <c r="S6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T6" t="s">
         <v>63</v>
@@ -1257,7 +1263,7 @@
         <v>127</v>
       </c>
       <c r="S7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T7" t="s">
         <v>63</v>
@@ -1309,7 +1315,7 @@
         <v>128</v>
       </c>
       <c r="S8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T8" t="s">
         <v>63</v>
@@ -1358,7 +1364,7 @@
         <v>121</v>
       </c>
       <c r="S9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T9" t="s">
         <v>63</v>
@@ -1412,7 +1418,7 @@
         <v>119</v>
       </c>
       <c r="S10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T10" t="s">
         <v>63</v>
@@ -1463,7 +1469,7 @@
         <v>120</v>
       </c>
       <c r="S11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T11" t="s">
         <v>63</v>
@@ -1517,7 +1523,7 @@
         <v>120</v>
       </c>
       <c r="S12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T12" t="s">
         <v>63</v>
@@ -1563,7 +1569,7 @@
         <v>115</v>
       </c>
       <c r="S13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T13" t="s">
         <v>63</v>
@@ -1620,7 +1626,7 @@
         <v>63</v>
       </c>
       <c r="U14" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="V14">
         <v>3</v>
@@ -1712,7 +1718,7 @@
         <v>117</v>
       </c>
       <c r="S16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T16" t="s">
         <v>63</v>
@@ -1763,7 +1769,7 @@
         <v>78</v>
       </c>
       <c r="S17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T17" t="s">
         <v>63</v>
@@ -1863,7 +1869,7 @@
         <v>125</v>
       </c>
       <c r="S19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T19" t="s">
         <v>63</v>
@@ -1914,7 +1920,7 @@
         <v>125</v>
       </c>
       <c r="S20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T20" t="s">
         <v>63</v>
@@ -1965,7 +1971,7 @@
         <v>125</v>
       </c>
       <c r="S21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T21" t="s">
         <v>63</v>
@@ -2101,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="O24" t="s">
         <v>132</v>
@@ -2114,6 +2120,9 @@
       </c>
       <c r="R24" t="s">
         <v>113</v>
+      </c>
+      <c r="S24" t="s">
+        <v>148</v>
       </c>
       <c r="T24" t="s">
         <v>63</v>
@@ -2163,7 +2172,13 @@
       <c r="R25" t="s">
         <v>110</v>
       </c>
+      <c r="S25" t="s">
+        <v>110</v>
+      </c>
       <c r="T25" t="s">
+        <v>63</v>
+      </c>
+      <c r="U25" t="s">
         <v>63</v>
       </c>
       <c r="V25">
@@ -2202,7 +2217,13 @@
       <c r="R26" t="s">
         <v>97</v>
       </c>
+      <c r="S26" t="s">
+        <v>150</v>
+      </c>
       <c r="T26" t="s">
+        <v>63</v>
+      </c>
+      <c r="U26" t="s">
         <v>63</v>
       </c>
       <c r="V26" t="e">
@@ -2241,7 +2262,13 @@
       <c r="R27" t="s">
         <v>126</v>
       </c>
+      <c r="S27" t="s">
+        <v>126</v>
+      </c>
       <c r="T27" t="s">
+        <v>63</v>
+      </c>
+      <c r="U27" t="s">
         <v>63</v>
       </c>
       <c r="V27" t="e">
@@ -2280,7 +2307,13 @@
       <c r="R28" t="s">
         <v>122</v>
       </c>
+      <c r="S28" t="s">
+        <v>122</v>
+      </c>
       <c r="T28" t="s">
+        <v>63</v>
+      </c>
+      <c r="U28" t="s">
         <v>63</v>
       </c>
       <c r="V28" t="e">

</xml_diff>

<commit_message>
fix(components): components library has been restructurated
the schematics components library, now footprints library WIP
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="624" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8FE5450-F4DA-49B1-8C7D-3BD98C45B8F4}"/>
+  <xr:revisionPtr revIDLastSave="659" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{081B037D-FB27-4047-9E67-8C63781A3AEB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Componentes" sheetId="1" r:id="rId1"/>
-    <sheet name="C.phoenix-c1 por modulo" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="C.phoenix-c1 por modulo" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="238">
   <si>
     <t>power input</t>
   </si>
@@ -478,12 +479,341 @@
   <si>
     <t>DIOM4336X24N</t>
   </si>
+  <si>
+    <t>Part Number (Design Item ID)</t>
+  </si>
+  <si>
+    <t>Descripción corta</t>
+  </si>
+  <si>
+    <r>
+      <t>Nombre de librería sugerido (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>.SchLib</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Diodo TVS</t>
+  </si>
+  <si>
+    <t>Diodo TVS 48V unidireccional DO-214AA</t>
+  </si>
+  <si>
+    <t>TVS_48V_DO214AA - SMBJ48D-M3/1</t>
+  </si>
+  <si>
+    <t>STM32G431CBU6</t>
+  </si>
+  <si>
+    <t>Microcontrolador</t>
+  </si>
+  <si>
+    <t>STM32G431C8T6 UFQFPN48 32bit MCU</t>
+  </si>
+  <si>
+    <t>MCU_STM32G431_UFQFPN48 - STM32G431CBU6</t>
+  </si>
+  <si>
+    <t>MAX15062AATA+T</t>
+  </si>
+  <si>
+    <t>Convertidor DC-DC</t>
+  </si>
+  <si>
+    <t>Step-Down 600mA Síncrono</t>
+  </si>
+  <si>
+    <t>DC-DC_MAX15062_ATA - MAX15062AATA+T</t>
+  </si>
+  <si>
+    <t>Conector</t>
+  </si>
+  <si>
+    <t>Conector XT60 macho</t>
+  </si>
+  <si>
+    <t>Conn_XT60PW-M - XT60PW-M</t>
+  </si>
+  <si>
+    <t>RT0603BRD07650RL</t>
+  </si>
+  <si>
+    <t>Resistencia</t>
+  </si>
+  <si>
+    <t>0603, 1%, 650Ω</t>
+  </si>
+  <si>
+    <t>Res_650_0603 - RT0603BRD07650RL</t>
+  </si>
+  <si>
+    <t>RC0603BR-104K7L</t>
+  </si>
+  <si>
+    <t>0603, 5%, 100kΩ</t>
+  </si>
+  <si>
+    <t>Res_100K_0603 - RC0603BR-104K7L</t>
+  </si>
+  <si>
+    <t>Resistencia shunt</t>
+  </si>
+  <si>
+    <t>0805, 2mΩ, 1%</t>
+  </si>
+  <si>
+    <t>Res_Shunt_2m_0805 - CSSH0805FT2L00</t>
+  </si>
+  <si>
+    <t>TSON 30V 3.8A</t>
+  </si>
+  <si>
+    <t>MOSFET_TSON_30V_3A - TPN19008QM_LQ</t>
+  </si>
+  <si>
+    <t>0603X473K1RACTU</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>0603 0.047uF 100V</t>
+  </si>
+  <si>
+    <t>Cap_100V_0u047_0603 - 0603X473K1RACTU</t>
+  </si>
+  <si>
+    <t>0805GC102JAT2A</t>
+  </si>
+  <si>
+    <t>0805 1nF 100V</t>
+  </si>
+  <si>
+    <t>Cap_100V_1n_0805 - 0805GC102JAT2A</t>
+  </si>
+  <si>
+    <t>0805GC105MAT2A</t>
+  </si>
+  <si>
+    <t>0805 1uF 6.3V</t>
+  </si>
+  <si>
+    <t>Cap_6V3_1u_0805 - 0805GC105MAT2A</t>
+  </si>
+  <si>
+    <t>Diodo Schottky</t>
+  </si>
+  <si>
+    <t>200 mA 1 V SOD-523</t>
+  </si>
+  <si>
+    <t>D_Schottky_200mA_1V_SOD523 - BAT41KFILM</t>
+  </si>
+  <si>
+    <t>MB6K1600BR3M</t>
+  </si>
+  <si>
+    <t>Puente rectificador</t>
+  </si>
+  <si>
+    <t>3.3uH 20% 1MHz Metal 0603</t>
+  </si>
+  <si>
+    <t>Ind_3u3_0603 - MB6K1600BR3M</t>
+  </si>
+  <si>
+    <t>AS5600-ASOM</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Sensor magnético de posición</t>
+  </si>
+  <si>
+    <t>Sensor_AS5600 - AS5600-ASOM</t>
+  </si>
+  <si>
+    <t>Conn_01x01</t>
+  </si>
+  <si>
+    <t>Header 1x1</t>
+  </si>
+  <si>
+    <t>Conn_1x1 - Conn_01x01</t>
+  </si>
+  <si>
+    <t>LPS4018-333MR</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>33uH, 20% Ferrita, 1515</t>
+  </si>
+  <si>
+    <t>Ind_33uH_1515 - LPS4018-333MR</t>
+  </si>
+  <si>
+    <t>DRV8323RSRTR</t>
+  </si>
+  <si>
+    <t>Driver 60V Trifásico 40-WQFN</t>
+  </si>
+  <si>
+    <t>Driver_3PH_DRV8323_WQFN - DRV8323RSRTR</t>
+  </si>
+  <si>
+    <t>CMP-17439-000151-1</t>
+  </si>
+  <si>
+    <t>Header 5x5 1.5MM</t>
+  </si>
+  <si>
+    <t>Conn_Header_5x5_1.5MM - CMP-17439-000151-1</t>
+  </si>
+  <si>
+    <t>GRJ31CC7ZAA475KE01K</t>
+  </si>
+  <si>
+    <t>4.7uF, 100V, 1206</t>
+  </si>
+  <si>
+    <t>Cap_100V_4u7_1206 - GRJ31CC7ZAA475KE01K</t>
+  </si>
+  <si>
+    <t>0.1uF, 6.3V, 0201</t>
+  </si>
+  <si>
+    <t>Cap_6V3_0u1_0201 - GRT033R60J104KE01J</t>
+  </si>
+  <si>
+    <t>1uF, 6.3V, 0805</t>
+  </si>
+  <si>
+    <t>Cap_6V3_1u_0805 - GCM21BC72A105KE36L</t>
+  </si>
+  <si>
+    <t>10uF, 6.3V, 0402</t>
+  </si>
+  <si>
+    <t>Cap_6V3_10u_0402 - GRM155R60J106ME05D</t>
+  </si>
+  <si>
+    <t>GRM033R60J474ME15D</t>
+  </si>
+  <si>
+    <t>0.47uF, 6.3V, 0201</t>
+  </si>
+  <si>
+    <t>Cap_6V3_0u47_0201 - GRM033R60J474ME15D</t>
+  </si>
+  <si>
+    <t>1uF, 6.3V, 0603</t>
+  </si>
+  <si>
+    <t>Cap_6V3_1u_0603 - GRM188R60J105KA01D</t>
+  </si>
+  <si>
+    <t>0.1uF, 100V, 0603</t>
+  </si>
+  <si>
+    <t>Cap_100V_0u1_0603 - GCJ188R72A104KA01D</t>
+  </si>
+  <si>
+    <t>0.1uF, 6.3V, 01005</t>
+  </si>
+  <si>
+    <t>Cap_6V3_0u1_01005 - GRM022R60J104ME15L</t>
+  </si>
+  <si>
+    <t>APT1608SURCK</t>
+  </si>
+  <si>
+    <t>LED rojo 0603</t>
+  </si>
+  <si>
+    <t>LED_Red_0603 - APT1608SURCK</t>
+  </si>
+  <si>
+    <t>AF024JR-0722KL</t>
+  </si>
+  <si>
+    <t>22kΩ, 1%, 0603</t>
+  </si>
+  <si>
+    <t>Res_22K_0603 - AF024JR-0722KL</t>
+  </si>
+  <si>
+    <t>22Ω, 5%, 0603</t>
+  </si>
+  <si>
+    <t>Res_22_0603 - RC0603JR-0722RL</t>
+  </si>
+  <si>
+    <t>XT30 macho</t>
+  </si>
+  <si>
+    <t>Conn_XT30PW-M - XT30PW-M</t>
+  </si>
+  <si>
+    <t>1uF, 25V, X7R, 0603</t>
+  </si>
+  <si>
+    <t>Cap_25V_1u_0603 - C1608X7R1E105K080AE</t>
+  </si>
+  <si>
+    <t>Arduino_PINS</t>
+  </si>
+  <si>
+    <t>Header simbólico</t>
+  </si>
+  <si>
+    <t>Pines para Arduino</t>
+  </si>
+  <si>
+    <t>Conn_Arduino_Header - Arduino_PINS</t>
+  </si>
+  <si>
+    <t>TH_UART</t>
+  </si>
+  <si>
+    <t>Header para UART</t>
+  </si>
+  <si>
+    <t>Conn_UART_Header - TH_UART</t>
+  </si>
+  <si>
+    <t>Modificado</t>
+  </si>
+  <si>
+    <t>Grilla</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,13 +865,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -557,7 +900,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -571,6 +914,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -579,6 +931,15 @@
   <dxfs count="6">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -597,15 +958,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -658,17 +1010,17 @@
     <tableColumn id="13" xr3:uid="{2B03112D-768E-4B24-BA12-EF1CD9491DBB}" name="NEW PCBLIbrary"/>
     <tableColumn id="12" xr3:uid="{66492975-40D9-428C-86A9-603CEEEB080E}" name="Sch  Corregido"/>
     <tableColumn id="11" xr3:uid="{F6CD5E74-C2A7-497A-977E-F83F137C4127}" name="FP Corregido"/>
-    <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="5" totalsRowDxfId="1">
+    <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F8E4DDA3-B94B-4AA6-A9F3-1C390E031E27}" name="Link" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{F8E4DDA3-B94B-4AA6-A9F3-1C390E031E27}" name="Link" dataDxfId="3">
       <calculatedColumnFormula>HYPERLINK("https://github.com/tu_repo","Ver repo")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3EB6D48B-B456-4C54-9366-899F34DB475D}" name="Precio unitario(USD)"/>
-    <tableColumn id="5" xr3:uid="{E2B14899-0F61-4692-90A3-AC74A17D725D}" name="CantX$(USD)" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{E2B14899-0F61-4692-90A3-AC74A17D725D}" name="CantX$(USD)" dataDxfId="2">
       <calculatedColumnFormula>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{81E0CD81-31E1-4B12-A1CA-8459D81315C8}" name="CantX$(CLP)" dataDxfId="2" totalsRowDxfId="0">
+    <tableColumn id="6" xr3:uid="{81E0CD81-31E1-4B12-A1CA-8459D81315C8}" name="CantX$(CLP)" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1010,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
   <dimension ref="A2:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="K2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
@@ -2246,6 +2598,598 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0F4C88-DBF5-4C06-9F1A-BD52F4E19CCD}">
+  <dimension ref="C6:H39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="53" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C8" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C25" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C35" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C37" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C39" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EDAD98-4A51-48B0-BAE4-039E551A8C8C}">
   <dimension ref="B2:I40"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix(footprints): footprints library has been restructurated
All the footprints components library has been finished
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="756" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8EFABEB-11D4-4199-8D6E-966F2D822314}"/>
+  <xr:revisionPtr revIDLastSave="792" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{014E555B-E676-43A7-B4C5-DD9BAD5443C9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Componentes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="265">
   <si>
     <t>power input</t>
   </si>
@@ -349,9 +349,6 @@
   </si>
   <si>
     <t>https://www.mouser.cl/ProductDetail/YAGEO/RC0603FR-104K7L?qs=sGAEpiMZZMtlubZbdhIBIHvQf5egq9lv0mk7h5hs6B0%3D</t>
-  </si>
-  <si>
-    <t>B82464P4333M000</t>
   </si>
   <si>
     <t>3.3 uh</t>
@@ -846,6 +843,51 @@
   </si>
   <si>
     <t>C01005-MURATA</t>
+  </si>
+  <si>
+    <t>C0201 - MURATA</t>
+  </si>
+  <si>
+    <t>C0402 - MURATA</t>
+  </si>
+  <si>
+    <t>C0603 - MURATA</t>
+  </si>
+  <si>
+    <t>C0603 - TDK</t>
+  </si>
+  <si>
+    <t>C0805 - 	KYOCERA</t>
+  </si>
+  <si>
+    <t>C0805 - MURATA</t>
+  </si>
+  <si>
+    <t>C1206 - MURATA</t>
+  </si>
+  <si>
+    <t>CONN - XT30PW</t>
+  </si>
+  <si>
+    <t>DDO-214AA (SMBJ) - VISHAY</t>
+  </si>
+  <si>
+    <t>L1515 - COILCRAFT</t>
+  </si>
+  <si>
+    <t>LED0603 - KINGBRIGHT</t>
+  </si>
+  <si>
+    <t>R0402 - YAGEO</t>
+  </si>
+  <si>
+    <t>R0603 - YAGEO</t>
+  </si>
+  <si>
+    <t>R0805 - SEI</t>
+  </si>
+  <si>
+    <t>DSOD-523 - STMicroelectronics</t>
   </si>
 </sst>
 </file>
@@ -1409,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
   <dimension ref="A2:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1428,7 +1470,8 @@
     <col min="14" max="15" width="17.44140625" customWidth="1"/>
     <col min="16" max="16" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.33203125" customWidth="1"/>
     <col min="21" max="21" width="12.5546875" customWidth="1"/>
     <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1499,7 +1542,7 @@
         <v>13</v>
       </c>
       <c r="O5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P5" t="s">
         <v>77</v>
@@ -1508,16 +1551,16 @@
         <v>70</v>
       </c>
       <c r="R5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V5" t="s">
         <v>37</v>
@@ -1546,22 +1589,22 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
+        <v>238</v>
+      </c>
+      <c r="O6" t="s">
         <v>239</v>
       </c>
-      <c r="O6" t="s">
-        <v>240</v>
-      </c>
       <c r="P6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q6" t="s">
         <v>63</v>
       </c>
       <c r="R6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="T6" t="s">
         <v>63</v>
@@ -1582,22 +1625,22 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q7" t="s">
         <v>63</v>
       </c>
       <c r="R7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="S7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T7" t="s">
         <v>63</v>
@@ -1625,22 +1668,22 @@
         <v>2</v>
       </c>
       <c r="N8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q8" t="s">
         <v>63</v>
       </c>
       <c r="R8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="S8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T8" t="s">
         <v>63</v>
@@ -1673,10 +1716,10 @@
         <v>63</v>
       </c>
       <c r="R9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="T9" t="s">
         <v>63</v>
@@ -1710,19 +1753,19 @@
         <v>31</v>
       </c>
       <c r="O10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q10" t="s">
         <v>63</v>
       </c>
       <c r="R10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="S10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T10" t="s">
         <v>63</v>
@@ -1758,19 +1801,22 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q11" t="s">
         <v>63</v>
       </c>
+      <c r="R11" t="s">
+        <v>250</v>
+      </c>
       <c r="S11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T11" t="s">
         <v>63</v>
@@ -1782,7 +1828,7 @@
         <v>5</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y11">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
@@ -1804,19 +1850,22 @@
         <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q12" t="s">
         <v>63</v>
       </c>
+      <c r="R12" t="s">
+        <v>250</v>
+      </c>
       <c r="S12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T12" t="s">
         <v>63</v>
@@ -1828,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Y12">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
@@ -1850,16 +1899,19 @@
         <v>32</v>
       </c>
       <c r="O13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q13" t="s">
         <v>63</v>
       </c>
+      <c r="R13" t="s">
+        <v>251</v>
+      </c>
       <c r="S13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T13" t="s">
         <v>63</v>
@@ -1898,7 +1950,7 @@
         <v>17</v>
       </c>
       <c r="O14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P14" t="s">
         <v>76</v>
@@ -1906,8 +1958,11 @@
       <c r="Q14" t="s">
         <v>63</v>
       </c>
+      <c r="R14" t="s">
+        <v>252</v>
+      </c>
       <c r="S14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T14" t="s">
         <v>63</v>
@@ -1946,7 +2001,7 @@
         <v>18</v>
       </c>
       <c r="O15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P15" t="s">
         <v>56</v>
@@ -1954,8 +2009,11 @@
       <c r="Q15" t="s">
         <v>63</v>
       </c>
+      <c r="R15" t="s">
+        <v>252</v>
+      </c>
       <c r="S15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T15" t="s">
         <v>63</v>
@@ -1994,16 +2052,19 @@
         <v>73</v>
       </c>
       <c r="O16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q16" t="s">
         <v>63</v>
       </c>
+      <c r="R16" t="s">
+        <v>252</v>
+      </c>
       <c r="S16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T16" t="s">
         <v>63</v>
@@ -2015,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Y16">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
@@ -2037,7 +2098,7 @@
         <v>19</v>
       </c>
       <c r="O17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P17" t="s">
         <v>82</v>
@@ -2045,8 +2106,11 @@
       <c r="Q17" t="s">
         <v>63</v>
       </c>
+      <c r="R17" t="s">
+        <v>253</v>
+      </c>
       <c r="S17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T17" t="s">
         <v>63</v>
@@ -2085,7 +2149,7 @@
         <v>83</v>
       </c>
       <c r="O18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P18" t="s">
         <v>84</v>
@@ -2093,8 +2157,11 @@
       <c r="Q18" t="s">
         <v>63</v>
       </c>
+      <c r="R18" t="s">
+        <v>254</v>
+      </c>
       <c r="S18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T18" t="s">
         <v>63</v>
@@ -2132,7 +2199,7 @@
         <v>74</v>
       </c>
       <c r="O19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P19" t="s">
         <v>72</v>
@@ -2140,8 +2207,11 @@
       <c r="Q19" t="s">
         <v>63</v>
       </c>
+      <c r="R19" t="s">
+        <v>254</v>
+      </c>
       <c r="S19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T19" t="s">
         <v>63</v>
@@ -2180,7 +2250,7 @@
         <v>15</v>
       </c>
       <c r="O20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P20" t="s">
         <v>75</v>
@@ -2188,8 +2258,11 @@
       <c r="Q20" t="s">
         <v>63</v>
       </c>
+      <c r="R20" t="s">
+        <v>255</v>
+      </c>
       <c r="S20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T20" t="s">
         <v>63</v>
@@ -2228,7 +2301,7 @@
         <v>29</v>
       </c>
       <c r="O21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P21" t="s">
         <v>78</v>
@@ -2236,8 +2309,11 @@
       <c r="Q21" t="s">
         <v>63</v>
       </c>
+      <c r="R21" t="s">
+        <v>256</v>
+      </c>
       <c r="S21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T21" t="s">
         <v>63</v>
@@ -2275,7 +2351,7 @@
         <v>14</v>
       </c>
       <c r="O22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P22" t="s">
         <v>14</v>
@@ -2283,8 +2359,11 @@
       <c r="Q22" t="s">
         <v>63</v>
       </c>
+      <c r="R22" t="s">
+        <v>257</v>
+      </c>
       <c r="S22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T22" t="s">
         <v>63</v>
@@ -2312,16 +2391,19 @@
         <v>36</v>
       </c>
       <c r="O23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q23" t="s">
         <v>63</v>
       </c>
+      <c r="R23" t="s">
+        <v>258</v>
+      </c>
       <c r="S23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T23" t="s">
         <v>63</v>
@@ -2352,19 +2434,19 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O24" t="s">
-        <v>119</v>
-      </c>
-      <c r="P24" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="Q24" t="s">
         <v>63</v>
       </c>
+      <c r="R24" t="s">
+        <v>259</v>
+      </c>
       <c r="S24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T24" t="s">
         <v>63</v>
@@ -2376,10 +2458,7 @@
         <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="W24" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/4qpAEMl","Mouser")</f>
-        <v>Mouser</v>
-      </c>
+      <c r="W24" s="1"/>
       <c r="X24" s="4">
         <v>1.59</v>
       </c>
@@ -2403,7 +2482,7 @@
         <v>40</v>
       </c>
       <c r="O25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P25" t="s">
         <v>90</v>
@@ -2411,8 +2490,11 @@
       <c r="Q25" t="s">
         <v>63</v>
       </c>
+      <c r="R25" t="s">
+        <v>260</v>
+      </c>
       <c r="S25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T25" t="s">
         <v>63</v>
@@ -2445,7 +2527,7 @@
         <v>22</v>
       </c>
       <c r="O26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P26" t="s">
         <v>80</v>
@@ -2453,8 +2535,11 @@
       <c r="Q26" t="s">
         <v>63</v>
       </c>
+      <c r="R26" t="s">
+        <v>261</v>
+      </c>
       <c r="S26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T26" t="s">
         <v>63</v>
@@ -2482,7 +2567,7 @@
         <v>33</v>
       </c>
       <c r="O27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P27" s="4" t="s">
         <v>91</v>
@@ -2490,8 +2575,11 @@
       <c r="Q27" t="s">
         <v>63</v>
       </c>
+      <c r="R27" t="s">
+        <v>262</v>
+      </c>
       <c r="S27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T27" t="s">
         <v>63</v>
@@ -2522,7 +2610,7 @@
         <v>24</v>
       </c>
       <c r="O28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P28" t="s">
         <v>85</v>
@@ -2530,8 +2618,11 @@
       <c r="Q28" t="s">
         <v>63</v>
       </c>
+      <c r="R28" t="s">
+        <v>262</v>
+      </c>
       <c r="S28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T28" t="s">
         <v>63</v>
@@ -2560,7 +2651,7 @@
         <v>26</v>
       </c>
       <c r="O29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P29" t="s">
         <v>89</v>
@@ -2568,8 +2659,11 @@
       <c r="Q29" t="s">
         <v>63</v>
       </c>
+      <c r="R29" t="s">
+        <v>262</v>
+      </c>
       <c r="S29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T29" t="s">
         <v>63</v>
@@ -2598,7 +2692,7 @@
         <v>21</v>
       </c>
       <c r="O30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P30" t="s">
         <v>55</v>
@@ -2606,8 +2700,11 @@
       <c r="Q30" t="s">
         <v>63</v>
       </c>
+      <c r="R30" t="s">
+        <v>263</v>
+      </c>
       <c r="S30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="T30" t="s">
         <v>63</v>
@@ -2636,7 +2733,7 @@
         <v>23</v>
       </c>
       <c r="O31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P31" t="s">
         <v>23</v>
@@ -2644,8 +2741,11 @@
       <c r="Q31" t="s">
         <v>63</v>
       </c>
+      <c r="R31" t="s">
+        <v>264</v>
+      </c>
       <c r="S31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T31" t="s">
         <v>63</v>
@@ -2671,22 +2771,22 @@
     </row>
     <row r="32" spans="5:26" x14ac:dyDescent="0.3">
       <c r="N32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q32" t="s">
         <v>63</v>
       </c>
       <c r="R32" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S32" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T32" t="s">
         <v>63</v>
@@ -2735,22 +2835,22 @@
   <sheetData>
     <row r="6" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C6" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2758,13 +2858,13 @@
         <v>36</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>63</v>
@@ -2772,30 +2872,30 @@
     </row>
     <row r="8" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>63</v>
@@ -2803,16 +2903,16 @@
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>63</v>
@@ -2820,16 +2920,16 @@
     </row>
     <row r="11" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C11" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>154</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>63</v>
@@ -2837,16 +2937,16 @@
     </row>
     <row r="12" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C12" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>63</v>
@@ -2857,13 +2957,13 @@
         <v>55</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>63</v>
@@ -2877,10 +2977,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>63</v>
@@ -2888,16 +2988,16 @@
     </row>
     <row r="15" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C15" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>63</v>
@@ -2905,16 +3005,16 @@
     </row>
     <row r="16" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>63</v>
@@ -2922,16 +3022,16 @@
     </row>
     <row r="17" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C17" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>63</v>
@@ -2942,13 +3042,13 @@
         <v>23</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>63</v>
@@ -2956,30 +3056,30 @@
     </row>
     <row r="19" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C19" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="20" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C20" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>63</v>
@@ -2987,16 +3087,16 @@
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>63</v>
@@ -3004,16 +3104,16 @@
     </row>
     <row r="22" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C22" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>190</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>63</v>
@@ -3021,16 +3121,16 @@
     </row>
     <row r="23" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C23" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>192</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>193</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>63</v>
@@ -3038,16 +3138,16 @@
     </row>
     <row r="24" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C24" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="F24" s="8" t="s">
         <v>195</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>196</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>63</v>
@@ -3055,16 +3155,16 @@
     </row>
     <row r="25" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C25" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>199</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>63</v>
@@ -3072,16 +3172,16 @@
     </row>
     <row r="26" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C26" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>201</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>63</v>
@@ -3092,13 +3192,13 @@
         <v>75</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>63</v>
@@ -3106,16 +3206,16 @@
     </row>
     <row r="28" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C28" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>204</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>205</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>63</v>
@@ -3123,16 +3223,16 @@
     </row>
     <row r="29" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C29" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>63</v>
@@ -3140,16 +3240,16 @@
     </row>
     <row r="30" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C30" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E30" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>210</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>63</v>
@@ -3160,13 +3260,13 @@
         <v>56</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E31" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>63</v>
@@ -3174,16 +3274,16 @@
     </row>
     <row r="32" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C32" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>214</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>63</v>
@@ -3191,16 +3291,16 @@
     </row>
     <row r="33" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C33" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>217</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>63</v>
@@ -3208,16 +3308,16 @@
     </row>
     <row r="34" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C34" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>63</v>
@@ -3228,13 +3328,13 @@
         <v>85</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E35" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>221</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>222</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>63</v>
@@ -3245,13 +3345,13 @@
         <v>14</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E36" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>63</v>
@@ -3262,13 +3362,13 @@
         <v>76</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>63</v>
@@ -3276,16 +3376,16 @@
     </row>
     <row r="38" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C38" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>63</v>
@@ -3293,16 +3393,16 @@
     </row>
     <row r="39" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C39" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>232</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3719,10 +3819,10 @@
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E37">
         <v>5</v>
@@ -3736,7 +3836,7 @@
         <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -3747,10 +3847,10 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -3761,10 +3861,10 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E40">
         <v>1</v>

</xml_diff>

<commit_message>
fix(schematics): schematics were revinculated to footprints
all the schematics has been revinculted to footprint respectly
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="792" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{014E555B-E676-43A7-B4C5-DD9BAD5443C9}"/>
+  <xr:revisionPtr revIDLastSave="838" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610783BF-7A1C-4BB5-989A-9AE1B17E1F66}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="246">
   <si>
     <t>power input</t>
   </si>
@@ -342,9 +342,6 @@
     <t>RT0603BRD07560RL</t>
   </si>
   <si>
-    <t>APT1608SURC</t>
-  </si>
-  <si>
     <t>RC0603FR-104K7L</t>
   </si>
   <si>
@@ -396,21 +393,9 @@
     <t>FP Corregido</t>
   </si>
   <si>
-    <t>SODFL1608X70N</t>
-  </si>
-  <si>
     <t>Sch  Corregido</t>
   </si>
   <si>
-    <t>NEW PCBLIbrary</t>
-  </si>
-  <si>
-    <t>INDPM104104X480N</t>
-  </si>
-  <si>
-    <t>LEDC1608X85N</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
@@ -429,46 +414,7 @@
     <t>INDUCTOR</t>
   </si>
   <si>
-    <t>RESC2013X06N</t>
-  </si>
-  <si>
-    <t>RESC1005X04N</t>
-  </si>
-  <si>
-    <t>CAPC2012X05N</t>
-  </si>
-  <si>
-    <t>CAPC1608X10N</t>
-  </si>
-  <si>
-    <t>CAPC0402X02L</t>
-  </si>
-  <si>
-    <t>CAPC2012X14N</t>
-  </si>
-  <si>
-    <t>CAPC1608X09N</t>
-  </si>
-  <si>
-    <t>CAPC3216X19N</t>
-  </si>
-  <si>
-    <t>CAPC1005X07N</t>
-  </si>
-  <si>
-    <t>CAPC0603X03N</t>
-  </si>
-  <si>
-    <t>CAPC0603X06N</t>
-  </si>
-  <si>
-    <t>RESC1608X06N</t>
-  </si>
-  <si>
     <t>XT60PW-M</t>
-  </si>
-  <si>
-    <t>DIOM4336X24N</t>
   </si>
   <si>
     <t>Part Number (Design Item ID)</t>
@@ -824,9 +770,6 @@
     <t>BUCK</t>
   </si>
   <si>
-    <t>CONN_XT30PWM</t>
-  </si>
-  <si>
     <t xml:space="preserve">8-TDFN </t>
   </si>
   <si>
@@ -854,9 +797,6 @@
     <t>C0603 - MURATA</t>
   </si>
   <si>
-    <t>C0603 - TDK</t>
-  </si>
-  <si>
     <t>C0805 - 	KYOCERA</t>
   </si>
   <si>
@@ -888,6 +828,9 @@
   </si>
   <si>
     <t>DSOD-523 - STMicroelectronics</t>
+  </si>
+  <si>
+    <t>C0603 - KEMET</t>
   </si>
 </sst>
 </file>
@@ -1085,18 +1028,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:Z33" totalsRowCount="1">
-  <autoFilter ref="N5:Z32" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N6:Z32">
-    <sortCondition ref="S5:S32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}" name="Tabla2" displayName="Tabla2" ref="N5:Y33" totalsRowCount="1">
+  <autoFilter ref="N5:Y32" xr:uid="{B1B482A5-D867-462B-9A42-5E02AF1BC0EA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N6:Y32">
+    <sortCondition ref="O5:O32"/>
   </sortState>
-  <tableColumns count="13">
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{2A8164C2-2FB7-4C23-97F1-2EB7091D5D63}" name="COMPONENTES"/>
     <tableColumn id="7" xr3:uid="{1B66CD5D-E06C-4FE7-9C8A-156F9A991661}" name="Tipo"/>
     <tableColumn id="9" xr3:uid="{916D2FE0-85EB-46DA-9799-D85CA8D5156F}" name="Part Number"/>
     <tableColumn id="8" xr3:uid="{B1046C3A-A1F3-421E-9436-C5BB3C6B237A}" name="Altium"/>
     <tableColumn id="10" xr3:uid="{0817AB30-E701-4F3F-93EE-84D6B2454E86}" name="Library Footprint"/>
-    <tableColumn id="13" xr3:uid="{2B03112D-768E-4B24-BA12-EF1CD9491DBB}" name="NEW PCBLIbrary"/>
     <tableColumn id="12" xr3:uid="{66492975-40D9-428C-86A9-603CEEEB080E}" name="Sch  Corregido"/>
     <tableColumn id="11" xr3:uid="{F6CD5E74-C2A7-497A-977E-F83F137C4127}" name="FP Corregido"/>
     <tableColumn id="2" xr3:uid="{E0C099EA-6525-4D7A-8A81-ABCE7DC1E501}" name="Cantidad" dataDxfId="5" totalsRowDxfId="1">
@@ -1118,8 +1060,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}" name="Tabla3" displayName="Tabla3" ref="Y2:Z3" totalsRowShown="0">
-  <autoFilter ref="Y2:Z3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}" name="Tabla3" displayName="Tabla3" ref="X2:Y3" totalsRowShown="0">
+  <autoFilter ref="X2:Y3" xr:uid="{E28B6582-852F-4E91-9FAF-A50541E24129}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6441C57D-BDB7-4FF4-9BC8-CECA7F77E429}" name="TOTAL(USD)">
       <calculatedColumnFormula>SUM(Tabla2[CantX$(USD)])</calculatedColumnFormula>
@@ -1449,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
-  <dimension ref="A2:Z33"/>
+  <dimension ref="A2:Y33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,43 +1413,42 @@
     <col min="16" max="16" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" customWidth="1"/>
-    <col min="21" max="21" width="12.5546875" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.88671875" customWidth="1"/>
-    <col min="24" max="24" width="20.109375" customWidth="1"/>
-    <col min="25" max="25" width="13.5546875" customWidth="1"/>
-    <col min="26" max="26" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.88671875" customWidth="1"/>
+    <col min="23" max="23" width="20.109375" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X2" t="s">
+        <v>39</v>
+      </c>
       <c r="Y2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="X3">
+        <f>SUM(Tabla2[CantX$(USD)])</f>
+        <v>25.51</v>
+      </c>
       <c r="Y3">
-        <f>SUM(Tabla2[CantX$(USD)])</f>
-        <v>27.540000000000003</v>
-      </c>
-      <c r="Z3">
         <f>ROUND(SUM(Tabla2[CantX$(CLP)]),0)</f>
-        <v>29706</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+        <v>27794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1542,7 +1483,7 @@
         <v>13</v>
       </c>
       <c r="O5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="P5" t="s">
         <v>77</v>
@@ -1551,34 +1492,31 @@
         <v>70</v>
       </c>
       <c r="R5" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="S5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="T5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="U5" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="V5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="X5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1589,32 +1527,26 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="O6" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="P6" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="Q6" t="s">
         <v>63</v>
       </c>
       <c r="R6" t="s">
-        <v>245</v>
-      </c>
-      <c r="S6" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="T6" t="s">
         <v>63</v>
       </c>
-      <c r="U6" t="s">
-        <v>63</v>
-      </c>
-      <c r="W6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1625,1188 +1557,1100 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>237</v>
+        <v>83</v>
       </c>
       <c r="O7" t="s">
-        <v>240</v>
+        <v>111</v>
       </c>
       <c r="P7" t="s">
-        <v>237</v>
+        <v>84</v>
       </c>
       <c r="Q7" t="s">
         <v>63</v>
       </c>
       <c r="R7" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="S7" t="s">
-        <v>246</v>
+        <v>63</v>
       </c>
       <c r="T7" t="s">
         <v>63</v>
       </c>
-      <c r="U7" t="s">
-        <v>63</v>
-      </c>
-      <c r="W7" s="1"/>
-      <c r="Z7">
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W7">
+        <v>0.1</v>
+      </c>
+      <c r="X7">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="Y7">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>282.55500000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8" t="s">
+        <v>111</v>
+      </c>
+      <c r="P8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" t="s">
+        <v>234</v>
+      </c>
+      <c r="S8" t="s">
+        <v>63</v>
+      </c>
+      <c r="T8" t="s">
+        <v>63</v>
+      </c>
+      <c r="U8">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>4</v>
+      </c>
+      <c r="V8" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W8">
+        <v>0.34</v>
+      </c>
+      <c r="X8">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>1.36</v>
+      </c>
+      <c r="Y8">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>1280.9160000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" t="s">
+        <v>111</v>
+      </c>
+      <c r="P9" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" t="s">
+        <v>245</v>
+      </c>
+      <c r="S9" t="s">
+        <v>63</v>
+      </c>
+      <c r="T9" t="s">
+        <v>63</v>
+      </c>
+      <c r="U9">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>1</v>
+      </c>
+      <c r="V9" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/47aSprm","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W9">
+        <v>0.44</v>
+      </c>
+      <c r="X9">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.44</v>
+      </c>
+      <c r="Y9">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>414.41399999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>63</v>
+      </c>
+      <c r="R10" t="s">
+        <v>233</v>
+      </c>
+      <c r="T10" t="s">
+        <v>63</v>
+      </c>
+      <c r="U10">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>1</v>
+      </c>
+      <c r="V10" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/43ubkLk","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W10">
+        <v>0.24</v>
+      </c>
+      <c r="X10">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.24</v>
+      </c>
+      <c r="Y10">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>226.04400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" t="s">
+        <v>111</v>
+      </c>
+      <c r="P11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>63</v>
+      </c>
+      <c r="R11" t="s">
+        <v>233</v>
+      </c>
+      <c r="S11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T11" t="s">
+        <v>63</v>
+      </c>
+      <c r="U11">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>1</v>
+      </c>
+      <c r="V11" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/47GKd25","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W11">
+        <v>0.16</v>
+      </c>
+      <c r="X11">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.16</v>
+      </c>
+      <c r="Y11">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>150.696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" t="s">
+        <v>111</v>
+      </c>
+      <c r="P12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>63</v>
+      </c>
+      <c r="R12" t="s">
+        <v>235</v>
+      </c>
+      <c r="S12" t="s">
+        <v>63</v>
+      </c>
+      <c r="T12" t="s">
+        <v>63</v>
+      </c>
+      <c r="U12">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>4</v>
+      </c>
+      <c r="V12" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/4oCNLrW","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W12">
+        <v>0.42</v>
+      </c>
+      <c r="X12">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>1.68</v>
+      </c>
+      <c r="Y12">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>1582.308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" t="s">
+        <v>111</v>
+      </c>
+      <c r="P13" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" t="s">
+        <v>236</v>
+      </c>
+      <c r="S13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" t="s">
+        <v>63</v>
+      </c>
+      <c r="U13">
+        <v>12</v>
+      </c>
+      <c r="V13" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W13">
+        <v>0.8</v>
+      </c>
+      <c r="X13">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="Y13">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>9041.760000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="N14" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" t="s">
+        <v>111</v>
+      </c>
+      <c r="P14" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>63</v>
+      </c>
+      <c r="R14" t="s">
+        <v>230</v>
+      </c>
+      <c r="S14" t="s">
+        <v>63</v>
+      </c>
+      <c r="T14" t="s">
+        <v>63</v>
+      </c>
+      <c r="U14">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>2</v>
+      </c>
+      <c r="V14" s="2" t="str">
+        <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W14">
+        <v>0.1</v>
+      </c>
+      <c r="X14">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y14">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>188.37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="N15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O15" t="s">
+        <v>111</v>
+      </c>
+      <c r="P15" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>63</v>
+      </c>
+      <c r="R15" t="s">
+        <v>231</v>
+      </c>
+      <c r="S15" t="s">
+        <v>63</v>
+      </c>
+      <c r="T15" t="s">
+        <v>63</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X15">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>1</v>
+      </c>
+      <c r="Y15">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>941.85</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" t="s">
+        <v>111</v>
+      </c>
+      <c r="P16" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>63</v>
+      </c>
+      <c r="R16" t="s">
+        <v>232</v>
+      </c>
+      <c r="S16" t="s">
+        <v>63</v>
+      </c>
+      <c r="T16" t="s">
+        <v>63</v>
+      </c>
+      <c r="U16">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
+        <v>3</v>
+      </c>
+      <c r="V16" s="2" t="str">
+        <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W16">
+        <v>0.1</v>
+      </c>
+      <c r="X16">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="Y16">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>282.55500000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" t="s">
+        <v>111</v>
+      </c>
+      <c r="P17" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>63</v>
+      </c>
+      <c r="R17" t="s">
+        <v>233</v>
+      </c>
+      <c r="S17" t="s">
+        <v>63</v>
+      </c>
+      <c r="T17" t="s">
+        <v>63</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="X17">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>1</v>
+      </c>
+      <c r="Y17">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>941.85</v>
+      </c>
+    </row>
+    <row r="18" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="N18" t="s">
+        <v>100</v>
+      </c>
+      <c r="O18" t="s">
+        <v>111</v>
+      </c>
+      <c r="P18" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>63</v>
+      </c>
+      <c r="R18" t="s">
+        <v>231</v>
+      </c>
+      <c r="S18" t="s">
+        <v>63</v>
+      </c>
+      <c r="T18" t="s">
+        <v>63</v>
+      </c>
+      <c r="U18">
+        <v>5</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X18">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>5</v>
+      </c>
+      <c r="Y18">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>4709.25</v>
+      </c>
+    </row>
+    <row r="19" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="N19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" t="s">
+        <v>110</v>
+      </c>
+      <c r="P19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>63</v>
+      </c>
+      <c r="R19" t="s">
+        <v>237</v>
+      </c>
+      <c r="S19" t="s">
+        <v>63</v>
+      </c>
+      <c r="T19" t="s">
+        <v>63</v>
+      </c>
+      <c r="V19" s="1"/>
+      <c r="W19">
+        <v>0.9</v>
+      </c>
+      <c r="Y19">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],942)</f>
+        <v>942</v>
+      </c>
+    </row>
+    <row r="20" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20">
         <v>2</v>
       </c>
-      <c r="G8">
+      <c r="N20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O20" t="s">
+        <v>109</v>
+      </c>
+      <c r="P20" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>63</v>
+      </c>
+      <c r="R20" t="s">
+        <v>240</v>
+      </c>
+      <c r="S20" t="s">
+        <v>63</v>
+      </c>
+      <c r="T20" t="s">
+        <v>63</v>
+      </c>
+      <c r="U20">
+        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
         <v>2</v>
       </c>
-      <c r="N8" t="s">
-        <v>236</v>
-      </c>
-      <c r="O8" t="s">
-        <v>242</v>
-      </c>
-      <c r="P8" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>63</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="V20" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/47slRYu","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W20">
+        <v>0.41</v>
+      </c>
+      <c r="X20">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.82</v>
+      </c>
+      <c r="Y20">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>772.31700000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="N21" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" t="s">
+        <v>109</v>
+      </c>
+      <c r="P21" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>63</v>
+      </c>
+      <c r="R21" t="s">
         <v>244</v>
       </c>
-      <c r="S8" t="s">
-        <v>244</v>
-      </c>
-      <c r="T8" t="s">
-        <v>63</v>
-      </c>
-      <c r="U8" t="s">
-        <v>63</v>
-      </c>
-      <c r="W8" s="1"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9">
+      <c r="S21" t="s">
+        <v>63</v>
+      </c>
+      <c r="T21" t="s">
+        <v>63</v>
+      </c>
+      <c r="V21" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/42XoOiu","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W21">
+        <v>0.34</v>
+      </c>
+      <c r="X21">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.34</v>
+      </c>
+      <c r="Y21">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>320.22900000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22">
+        <v>12</v>
+      </c>
+      <c r="N22" t="s">
+        <v>36</v>
+      </c>
+      <c r="O22" t="s">
+        <v>109</v>
+      </c>
+      <c r="P22" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>63</v>
+      </c>
+      <c r="R22" t="s">
+        <v>238</v>
+      </c>
+      <c r="S22" t="s">
+        <v>63</v>
+      </c>
+      <c r="T22" t="s">
+        <v>63</v>
+      </c>
+      <c r="V22" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/3Wle1em","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W22">
+        <v>0.34</v>
+      </c>
+      <c r="Y22">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>941.85</v>
+      </c>
+    </row>
+    <row r="23" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L23">
         <v>1</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N23" t="s">
+        <v>220</v>
+      </c>
+      <c r="O23" t="s">
+        <v>221</v>
+      </c>
+      <c r="P23" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>63</v>
+      </c>
+      <c r="R23" t="s">
+        <v>226</v>
+      </c>
+      <c r="S23" t="s">
+        <v>63</v>
+      </c>
+      <c r="T23" t="s">
+        <v>63</v>
+      </c>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="N24" t="s">
+        <v>161</v>
+      </c>
+      <c r="O24" t="s">
+        <v>223</v>
+      </c>
+      <c r="P24" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>63</v>
+      </c>
+      <c r="R24" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="S24" t="s">
+        <v>63</v>
+      </c>
+      <c r="T24" t="s">
+        <v>63</v>
+      </c>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="N25" t="s">
+        <v>92</v>
+      </c>
+      <c r="O25" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>63</v>
+      </c>
+      <c r="R25" t="s">
+        <v>239</v>
+      </c>
+      <c r="S25" t="s">
+        <v>63</v>
+      </c>
+      <c r="T25" t="s">
+        <v>63</v>
+      </c>
+      <c r="V25" s="1"/>
+      <c r="W25" s="4">
+        <v>1.59</v>
+      </c>
+      <c r="X25">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>1.59</v>
+      </c>
+      <c r="Y25">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>1497.5415</v>
+      </c>
+    </row>
+    <row r="26" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="N26" t="s">
+        <v>219</v>
+      </c>
+      <c r="O26" t="s">
+        <v>222</v>
+      </c>
+      <c r="P26" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>63</v>
+      </c>
+      <c r="R26" t="s">
+        <v>227</v>
+      </c>
+      <c r="S26" t="s">
+        <v>63</v>
+      </c>
+      <c r="T26" t="s">
+        <v>63</v>
+      </c>
+      <c r="V26" s="1"/>
+      <c r="Y26">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>941.85</v>
+      </c>
+    </row>
+    <row r="27" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
         <v>20</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O27" t="s">
         <v>58</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P27" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" t="s">
-        <v>63</v>
-      </c>
-      <c r="R9" t="s">
-        <v>248</v>
-      </c>
-      <c r="S9" t="s">
-        <v>248</v>
-      </c>
-      <c r="T9" t="s">
-        <v>63</v>
-      </c>
-      <c r="U9" t="s">
-        <v>63</v>
-      </c>
-      <c r="W9" s="1" t="str">
+      <c r="Q27" t="s">
+        <v>63</v>
+      </c>
+      <c r="R27" t="s">
+        <v>229</v>
+      </c>
+      <c r="S27" t="s">
+        <v>63</v>
+      </c>
+      <c r="T27" t="s">
+        <v>63</v>
+      </c>
+      <c r="V27" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/3Jxp5Cd","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="X9">
+      <c r="W27">
         <v>1.1100000000000001</v>
       </c>
-      <c r="Z9">
+      <c r="Y27">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>941.85</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" t="s">
-        <v>116</v>
-      </c>
-      <c r="P10" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>63</v>
-      </c>
-      <c r="R10" t="s">
-        <v>249</v>
-      </c>
-      <c r="S10" t="s">
-        <v>123</v>
-      </c>
-      <c r="T10" t="s">
-        <v>63</v>
-      </c>
-      <c r="U10" t="s">
-        <v>63</v>
-      </c>
-      <c r="V10">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>1</v>
-      </c>
-      <c r="W10" s="2" t="str">
-        <f>HYPERLINK("https://mou.sr/4owREP0","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X10">
-        <v>0.1</v>
-      </c>
-      <c r="Y10">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z10">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>94.185000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
-        <v>101</v>
-      </c>
-      <c r="O11" t="s">
-        <v>116</v>
-      </c>
-      <c r="P11" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>63</v>
-      </c>
-      <c r="R11" t="s">
-        <v>250</v>
-      </c>
-      <c r="S11" t="s">
-        <v>128</v>
-      </c>
-      <c r="T11" t="s">
-        <v>63</v>
-      </c>
-      <c r="U11" t="s">
-        <v>63</v>
-      </c>
-      <c r="V11">
-        <v>5</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y11">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>5</v>
-      </c>
-      <c r="Z11">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>4709.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="N12" t="s">
-        <v>99</v>
-      </c>
-      <c r="O12" t="s">
-        <v>116</v>
-      </c>
-      <c r="P12" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>63</v>
-      </c>
-      <c r="R12" t="s">
-        <v>250</v>
-      </c>
-      <c r="S12" t="s">
-        <v>129</v>
-      </c>
-      <c r="T12" t="s">
-        <v>63</v>
-      </c>
-      <c r="U12" t="s">
-        <v>63</v>
-      </c>
-      <c r="V12">
-        <v>1</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y12">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1</v>
-      </c>
-      <c r="Z12">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>941.85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O13" t="s">
-        <v>116</v>
-      </c>
-      <c r="P13" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>63</v>
-      </c>
-      <c r="R13" t="s">
-        <v>251</v>
-      </c>
-      <c r="S13" t="s">
-        <v>127</v>
-      </c>
-      <c r="T13" t="s">
-        <v>63</v>
-      </c>
-      <c r="U13" t="s">
-        <v>63</v>
-      </c>
-      <c r="V13">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>1</v>
-      </c>
-      <c r="W13" s="2" t="str">
-        <f>HYPERLINK("https://mou.sr/4qt9N1T","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X13">
-        <v>0.1</v>
-      </c>
-      <c r="Y13">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z13">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>94.185000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E14" t="s">
+    <row r="28" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
         <v>22</v>
       </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="N14" t="s">
-        <v>17</v>
-      </c>
-      <c r="O14" t="s">
-        <v>116</v>
-      </c>
-      <c r="P14" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>63</v>
-      </c>
-      <c r="R14" t="s">
-        <v>252</v>
-      </c>
-      <c r="S14" t="s">
-        <v>125</v>
-      </c>
-      <c r="T14" t="s">
-        <v>63</v>
-      </c>
-      <c r="U14" t="s">
-        <v>63</v>
-      </c>
-      <c r="V14">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>2</v>
-      </c>
-      <c r="W14" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/43ubkLk","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X14">
-        <v>0.24</v>
-      </c>
-      <c r="Y14">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.48</v>
-      </c>
-      <c r="Z14">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>452.08800000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15">
-        <v>6</v>
-      </c>
-      <c r="N15" t="s">
-        <v>18</v>
-      </c>
-      <c r="O15" t="s">
-        <v>116</v>
-      </c>
-      <c r="P15" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>63</v>
-      </c>
-      <c r="R15" t="s">
-        <v>252</v>
-      </c>
-      <c r="S15" t="s">
-        <v>125</v>
-      </c>
-      <c r="T15" t="s">
-        <v>63</v>
-      </c>
-      <c r="U15" t="s">
-        <v>63</v>
-      </c>
-      <c r="V15">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>6</v>
-      </c>
-      <c r="W15" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47GKd25","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X15">
-        <v>0.16</v>
-      </c>
-      <c r="Y15">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.96</v>
-      </c>
-      <c r="Z15">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>904.17600000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="N16" t="s">
-        <v>73</v>
-      </c>
-      <c r="O16" t="s">
-        <v>116</v>
-      </c>
-      <c r="P16" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>63</v>
-      </c>
-      <c r="R16" t="s">
-        <v>252</v>
-      </c>
-      <c r="S16" t="s">
-        <v>125</v>
-      </c>
-      <c r="T16" t="s">
-        <v>63</v>
-      </c>
-      <c r="U16" t="s">
-        <v>63</v>
-      </c>
-      <c r="V16">
-        <v>1</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y16">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1</v>
-      </c>
-      <c r="Z16">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>941.85</v>
-      </c>
-    </row>
-    <row r="17" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="N17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" t="s">
-        <v>116</v>
-      </c>
-      <c r="P17" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>63</v>
-      </c>
-      <c r="R17" t="s">
-        <v>253</v>
-      </c>
-      <c r="S17" t="s">
-        <v>122</v>
-      </c>
-      <c r="T17" t="s">
-        <v>63</v>
-      </c>
-      <c r="U17" t="s">
-        <v>63</v>
-      </c>
-      <c r="V17">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>3</v>
-      </c>
-      <c r="W17" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47aSprm","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X17">
-        <v>0.44</v>
-      </c>
-      <c r="Y17">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.32</v>
-      </c>
-      <c r="Z17">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>1243.2420000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18">
-        <v>3</v>
-      </c>
-      <c r="N18" t="s">
-        <v>83</v>
-      </c>
-      <c r="O18" t="s">
-        <v>116</v>
-      </c>
-      <c r="P18" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>63</v>
-      </c>
-      <c r="R18" t="s">
-        <v>254</v>
-      </c>
-      <c r="S18" t="s">
-        <v>121</v>
-      </c>
-      <c r="T18" t="s">
-        <v>63</v>
-      </c>
-      <c r="U18" t="s">
-        <v>63</v>
-      </c>
-      <c r="V18">
-        <v>3</v>
-      </c>
-      <c r="W18" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47cPcHL","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X18">
-        <v>0.1</v>
-      </c>
-      <c r="Y18">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="Z18">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>282.55500000000006</v>
-      </c>
-    </row>
-    <row r="19" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19">
-        <v>3</v>
-      </c>
-      <c r="N19" t="s">
-        <v>74</v>
-      </c>
-      <c r="O19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P19" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>63</v>
-      </c>
-      <c r="R19" t="s">
-        <v>254</v>
-      </c>
-      <c r="S19" t="s">
-        <v>121</v>
-      </c>
-      <c r="T19" t="s">
-        <v>63</v>
-      </c>
-      <c r="U19" t="s">
-        <v>63</v>
-      </c>
-      <c r="V19">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>3</v>
-      </c>
-      <c r="W19" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3JzqjNg","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X19">
-        <v>0.34</v>
-      </c>
-      <c r="Y19">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>1.02</v>
-      </c>
-      <c r="Z19">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>960.68700000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
-      </c>
-      <c r="N20" t="s">
-        <v>15</v>
-      </c>
-      <c r="O20" t="s">
-        <v>116</v>
-      </c>
-      <c r="P20" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>63</v>
-      </c>
-      <c r="R20" t="s">
-        <v>255</v>
-      </c>
-      <c r="S20" t="s">
-        <v>124</v>
-      </c>
-      <c r="T20" t="s">
-        <v>63</v>
-      </c>
-      <c r="U20" t="s">
-        <v>63</v>
-      </c>
-      <c r="V20">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>2</v>
-      </c>
-      <c r="W20" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/4oCNLrW","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X20">
-        <v>0.42</v>
-      </c>
-      <c r="Y20">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.84</v>
-      </c>
-      <c r="Z20">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>791.154</v>
-      </c>
-    </row>
-    <row r="21" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="J21">
-        <v>2</v>
-      </c>
-      <c r="N21" t="s">
-        <v>29</v>
-      </c>
-      <c r="O21" t="s">
-        <v>116</v>
-      </c>
-      <c r="P21" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>63</v>
-      </c>
-      <c r="R21" t="s">
-        <v>256</v>
-      </c>
-      <c r="S21" t="s">
-        <v>126</v>
-      </c>
-      <c r="T21" t="s">
-        <v>63</v>
-      </c>
-      <c r="U21" t="s">
-        <v>63</v>
-      </c>
-      <c r="V21">
-        <v>12</v>
-      </c>
-      <c r="W21" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3WUpj9x","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X21">
-        <v>0.8</v>
-      </c>
-      <c r="Y21">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>9.6000000000000014</v>
-      </c>
-      <c r="Z21">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>9041.760000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22">
-        <v>12</v>
-      </c>
-      <c r="N22" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" t="s">
-        <v>115</v>
-      </c>
-      <c r="P22" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R22" t="s">
-        <v>257</v>
-      </c>
-      <c r="S22" t="s">
-        <v>243</v>
-      </c>
-      <c r="T22" t="s">
-        <v>63</v>
-      </c>
-      <c r="U22" t="s">
-        <v>63</v>
-      </c>
-      <c r="W22" s="1"/>
-      <c r="X22">
-        <v>0.9</v>
-      </c>
-      <c r="Z22">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],942)</f>
-        <v>942</v>
-      </c>
-    </row>
-    <row r="23" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>31</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="N23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O23" t="s">
-        <v>114</v>
-      </c>
-      <c r="P23" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>63</v>
-      </c>
-      <c r="R23" t="s">
-        <v>258</v>
-      </c>
-      <c r="S23" t="s">
-        <v>132</v>
-      </c>
-      <c r="T23" t="s">
-        <v>63</v>
-      </c>
-      <c r="U23" t="s">
-        <v>63</v>
-      </c>
-      <c r="W23" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/3Wle1em","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X23">
-        <v>0.34</v>
-      </c>
-      <c r="Z23">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>941.85</v>
-      </c>
-    </row>
-    <row r="24" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="N24" t="s">
-        <v>93</v>
-      </c>
-      <c r="O24" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>63</v>
-      </c>
-      <c r="R24" t="s">
-        <v>259</v>
-      </c>
-      <c r="S24" t="s">
-        <v>111</v>
-      </c>
-      <c r="T24" t="s">
-        <v>63</v>
-      </c>
-      <c r="U24" t="s">
-        <v>63</v>
-      </c>
-      <c r="V24">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>2</v>
-      </c>
-      <c r="W24" s="1"/>
-      <c r="X24" s="4">
-        <v>1.59</v>
-      </c>
-      <c r="Y24">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>3.18</v>
-      </c>
-      <c r="Z24">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>2995.0830000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="E25" t="s">
-        <v>33</v>
-      </c>
-      <c r="L25">
-        <v>2</v>
-      </c>
-      <c r="N25" t="s">
-        <v>40</v>
-      </c>
-      <c r="O25" t="s">
-        <v>114</v>
-      </c>
-      <c r="P25" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>63</v>
-      </c>
-      <c r="R25" t="s">
-        <v>260</v>
-      </c>
-      <c r="S25" t="s">
+      <c r="O28" t="s">
         <v>112</v>
       </c>
-      <c r="T25" t="s">
-        <v>63</v>
-      </c>
-      <c r="U25" t="s">
-        <v>63</v>
-      </c>
-      <c r="V25">
-        <f>SUM(Tabla1[[#This Row],[Power Input(MAX15062AATA+T )]:[AS5600 ASOM]])</f>
-        <v>2</v>
-      </c>
-      <c r="W25" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47slRYu","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X25">
-        <v>0.41</v>
-      </c>
-      <c r="Y25">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.82</v>
-      </c>
-      <c r="Z25">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>772.31700000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="N26" t="s">
-        <v>22</v>
-      </c>
-      <c r="O26" t="s">
-        <v>117</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="P28" t="s">
         <v>80</v>
       </c>
-      <c r="Q26" t="s">
-        <v>63</v>
-      </c>
-      <c r="R26" t="s">
-        <v>261</v>
-      </c>
-      <c r="S26" t="s">
-        <v>120</v>
-      </c>
-      <c r="T26" t="s">
-        <v>63</v>
-      </c>
-      <c r="U26" t="s">
-        <v>63</v>
-      </c>
-      <c r="W26" s="2" t="s">
+      <c r="Q28" t="s">
+        <v>63</v>
+      </c>
+      <c r="R28" t="s">
+        <v>241</v>
+      </c>
+      <c r="S28" t="s">
+        <v>63</v>
+      </c>
+      <c r="T28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="X26">
+      <c r="W28">
         <v>0.18</v>
       </c>
-      <c r="Y26">
+      <c r="X28">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.18</v>
       </c>
-      <c r="Z26">
+      <c r="Y28">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>169.53299999999999</v>
       </c>
     </row>
-    <row r="27" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="N27" t="s">
+    <row r="29" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="N29" t="s">
+        <v>21</v>
+      </c>
+      <c r="O29" t="s">
+        <v>112</v>
+      </c>
+      <c r="P29" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>63</v>
+      </c>
+      <c r="R29" t="s">
+        <v>243</v>
+      </c>
+      <c r="T29" t="s">
+        <v>63</v>
+      </c>
+      <c r="V29" s="1" t="str">
+        <f>HYPERLINK("https://mou.sr/47oFwIR","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="W29">
+        <v>0.6</v>
+      </c>
+      <c r="X29">
+        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
+        <v>0.6</v>
+      </c>
+      <c r="Y29">
+        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
+        <v>565.11</v>
+      </c>
+    </row>
+    <row r="30" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="N30" t="s">
         <v>33</v>
       </c>
-      <c r="O27" t="s">
-        <v>117</v>
-      </c>
-      <c r="P27" s="4" t="s">
+      <c r="O30" t="s">
+        <v>112</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>63</v>
+      </c>
+      <c r="R30" t="s">
+        <v>242</v>
+      </c>
+      <c r="S30" t="s">
+        <v>63</v>
+      </c>
+      <c r="T30" t="s">
+        <v>63</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="V30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Q27" t="s">
-        <v>63</v>
-      </c>
-      <c r="R27" t="s">
-        <v>262</v>
-      </c>
-      <c r="S27" t="s">
-        <v>130</v>
-      </c>
-      <c r="T27" t="s">
-        <v>63</v>
-      </c>
-      <c r="U27" t="s">
-        <v>63</v>
-      </c>
-      <c r="V27">
-        <v>1</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="X27">
+      <c r="W30">
         <v>0.32</v>
       </c>
-      <c r="Y27">
+      <c r="X30">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.32</v>
       </c>
-      <c r="Z27">
+      <c r="Y30">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>301.392</v>
       </c>
     </row>
-    <row r="28" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="N28" t="s">
+    <row r="31" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="N31" t="s">
         <v>24</v>
       </c>
-      <c r="O28" t="s">
-        <v>117</v>
-      </c>
-      <c r="P28" t="s">
+      <c r="O31" t="s">
+        <v>112</v>
+      </c>
+      <c r="P31" t="s">
         <v>85</v>
       </c>
-      <c r="Q28" t="s">
-        <v>63</v>
-      </c>
-      <c r="R28" t="s">
-        <v>262</v>
-      </c>
-      <c r="S28" t="s">
-        <v>130</v>
-      </c>
-      <c r="T28" t="s">
-        <v>63</v>
-      </c>
-      <c r="U28" t="s">
-        <v>63</v>
-      </c>
-      <c r="W28" s="1" t="str">
+      <c r="Q31" t="s">
+        <v>63</v>
+      </c>
+      <c r="R31" t="s">
+        <v>242</v>
+      </c>
+      <c r="S31" t="s">
+        <v>63</v>
+      </c>
+      <c r="T31" t="s">
+        <v>63</v>
+      </c>
+      <c r="V31" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/47bBWDf","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="X28">
+      <c r="W31">
         <v>0.15</v>
       </c>
-      <c r="Y28">
+      <c r="X31">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.15</v>
       </c>
-      <c r="Z28">
+      <c r="Y31">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>141.2775</v>
       </c>
     </row>
-    <row r="29" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="N29" t="s">
+    <row r="32" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="N32" t="s">
         <v>26</v>
       </c>
-      <c r="O29" t="s">
-        <v>117</v>
-      </c>
-      <c r="P29" t="s">
+      <c r="O32" t="s">
+        <v>112</v>
+      </c>
+      <c r="P32" t="s">
         <v>89</v>
       </c>
-      <c r="Q29" t="s">
-        <v>63</v>
-      </c>
-      <c r="R29" t="s">
-        <v>262</v>
-      </c>
-      <c r="S29" t="s">
-        <v>130</v>
-      </c>
-      <c r="T29" t="s">
-        <v>63</v>
-      </c>
-      <c r="U29" t="s">
-        <v>63</v>
-      </c>
-      <c r="W29" s="1" t="str">
+      <c r="Q32" t="s">
+        <v>63</v>
+      </c>
+      <c r="R32" t="s">
+        <v>242</v>
+      </c>
+      <c r="S32" t="s">
+        <v>63</v>
+      </c>
+      <c r="T32" t="s">
+        <v>63</v>
+      </c>
+      <c r="V32" s="1" t="str">
         <f>HYPERLINK("https://mou.sr/48K3Qr8","Mouser")</f>
         <v>Mouser</v>
       </c>
-      <c r="X29">
+      <c r="W32">
         <v>0.23</v>
       </c>
-      <c r="Y29">
+      <c r="X32">
         <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
         <v>0.23</v>
       </c>
-      <c r="Z29">
+      <c r="Y32">
         <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
         <v>216.62550000000002</v>
       </c>
     </row>
-    <row r="30" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="N30" t="s">
-        <v>21</v>
-      </c>
-      <c r="O30" t="s">
-        <v>117</v>
-      </c>
-      <c r="P30" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>63</v>
-      </c>
-      <c r="R30" t="s">
-        <v>263</v>
-      </c>
-      <c r="S30" t="s">
-        <v>119</v>
-      </c>
-      <c r="T30" t="s">
-        <v>63</v>
-      </c>
-      <c r="U30" t="s">
-        <v>63</v>
-      </c>
-      <c r="W30" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/47oFwIR","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X30">
-        <v>0.6</v>
-      </c>
-      <c r="Y30">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.6</v>
-      </c>
-      <c r="Z30">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>565.11</v>
-      </c>
-    </row>
-    <row r="31" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="N31" t="s">
-        <v>23</v>
-      </c>
-      <c r="O31" t="s">
-        <v>114</v>
-      </c>
-      <c r="P31" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>63</v>
-      </c>
-      <c r="R31" t="s">
-        <v>264</v>
-      </c>
-      <c r="S31" t="s">
-        <v>108</v>
-      </c>
-      <c r="T31" t="s">
-        <v>63</v>
-      </c>
-      <c r="U31" t="s">
-        <v>63</v>
-      </c>
-      <c r="W31" s="1" t="str">
-        <f>HYPERLINK("https://mou.sr/42XoOiu","Mouser")</f>
-        <v>Mouser</v>
-      </c>
-      <c r="X31">
-        <v>0.34</v>
-      </c>
-      <c r="Y31">
-        <f>PRODUCT(Tabla2[[#This Row],[Cantidad]],Tabla2[[#This Row],[Precio unitario(USD)]])</f>
-        <v>0.34</v>
-      </c>
-      <c r="Z31">
-        <f>PRODUCT(Tabla2[[#This Row],[CantX$(USD)]],941.85)</f>
-        <v>320.22900000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="5:26" x14ac:dyDescent="0.3">
-      <c r="N32" t="s">
-        <v>179</v>
-      </c>
-      <c r="O32" t="s">
-        <v>241</v>
-      </c>
-      <c r="P32" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>63</v>
-      </c>
-      <c r="R32" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="S32" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="T32" t="s">
-        <v>63</v>
-      </c>
-      <c r="U32" t="s">
-        <v>63</v>
-      </c>
-      <c r="W32" s="1"/>
-    </row>
-    <row r="33" spans="22:26" x14ac:dyDescent="0.3">
-      <c r="V33" s="6"/>
-      <c r="Z33" s="3"/>
+    <row r="33" spans="21:25" x14ac:dyDescent="0.3">
+      <c r="U33" s="6"/>
+      <c r="Y33" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W26" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
-    <hyperlink ref="W11" r:id="rId2" xr:uid="{B765BA37-3C00-40F5-AEDD-838B98A4DF8E}"/>
-    <hyperlink ref="W16" r:id="rId3" xr:uid="{B0DD47A4-DB96-49FA-9651-714D11187895}"/>
-    <hyperlink ref="W12" r:id="rId4" xr:uid="{23FAA789-D6A4-48F6-B5EA-A3B0AFCD0314}"/>
-    <hyperlink ref="W27" r:id="rId5" xr:uid="{3AFEECC7-F076-4F50-A9F6-AB0039D9AEF1}"/>
+    <hyperlink ref="V28" r:id="rId1" xr:uid="{155DAB3D-C7B6-4D36-AC1F-62B6A9BEF3AD}"/>
+    <hyperlink ref="V18" r:id="rId2" xr:uid="{B765BA37-3C00-40F5-AEDD-838B98A4DF8E}"/>
+    <hyperlink ref="V17" r:id="rId3" xr:uid="{B0DD47A4-DB96-49FA-9651-714D11187895}"/>
+    <hyperlink ref="V15" r:id="rId4" xr:uid="{23FAA789-D6A4-48F6-B5EA-A3B0AFCD0314}"/>
+    <hyperlink ref="V30" r:id="rId5" xr:uid="{3AFEECC7-F076-4F50-A9F6-AB0039D9AEF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
@@ -2835,22 +2679,22 @@
   <sheetData>
     <row r="6" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C6" s="7" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2858,13 +2702,13 @@
         <v>36</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>63</v>
@@ -2872,30 +2716,30 @@
     </row>
     <row r="8" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>63</v>
@@ -2903,16 +2747,16 @@
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>149</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>63</v>
@@ -2920,16 +2764,16 @@
     </row>
     <row r="11" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C11" s="8" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>63</v>
@@ -2937,16 +2781,16 @@
     </row>
     <row r="12" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C12" s="8" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>63</v>
@@ -2957,13 +2801,13 @@
         <v>55</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>63</v>
@@ -2977,10 +2821,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>63</v>
@@ -2988,16 +2832,16 @@
     </row>
     <row r="15" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C15" s="8" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>63</v>
@@ -3005,16 +2849,16 @@
     </row>
     <row r="16" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>63</v>
@@ -3022,16 +2866,16 @@
     </row>
     <row r="17" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C17" s="8" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>63</v>
@@ -3042,13 +2886,13 @@
         <v>23</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>63</v>
@@ -3056,30 +2900,30 @@
     </row>
     <row r="19" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C19" s="9" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C20" s="8" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>63</v>
@@ -3087,16 +2931,16 @@
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="8" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>63</v>
@@ -3104,16 +2948,16 @@
     </row>
     <row r="22" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C22" s="8" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>63</v>
@@ -3121,16 +2965,16 @@
     </row>
     <row r="23" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C23" s="8" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>63</v>
@@ -3138,16 +2982,16 @@
     </row>
     <row r="24" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C24" s="8" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>63</v>
@@ -3155,16 +2999,16 @@
     </row>
     <row r="25" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C25" s="8" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>63</v>
@@ -3172,16 +3016,16 @@
     </row>
     <row r="26" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C26" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>63</v>
@@ -3192,13 +3036,13 @@
         <v>75</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>63</v>
@@ -3206,16 +3050,16 @@
     </row>
     <row r="28" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C28" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>63</v>
@@ -3223,16 +3067,16 @@
     </row>
     <row r="29" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C29" s="8" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>63</v>
@@ -3240,16 +3084,16 @@
     </row>
     <row r="30" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C30" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>63</v>
@@ -3260,13 +3104,13 @@
         <v>56</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>63</v>
@@ -3274,16 +3118,16 @@
     </row>
     <row r="32" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C32" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>63</v>
@@ -3291,16 +3135,16 @@
     </row>
     <row r="33" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C33" s="8" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>63</v>
@@ -3308,16 +3152,16 @@
     </row>
     <row r="34" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C34" s="8" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>63</v>
@@ -3328,13 +3172,13 @@
         <v>85</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>63</v>
@@ -3345,13 +3189,13 @@
         <v>14</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>63</v>
@@ -3362,13 +3206,13 @@
         <v>76</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>63</v>
@@ -3376,16 +3220,16 @@
     </row>
     <row r="38" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C38" s="8" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>63</v>
@@ -3393,16 +3237,16 @@
     </row>
     <row r="39" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C39" s="8" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3819,10 +3663,10 @@
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E37">
         <v>5</v>
@@ -3836,7 +3680,7 @@
         <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -3847,10 +3691,10 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -3861,10 +3705,10 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E40">
         <v>1</v>

</xml_diff>

<commit_message>
fix(schematics): all schematics has been fixed with the new components
</commit_message>
<xml_diff>
--- a/docs/passive components.xlsx
+++ b/docs/passive components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/rodrigo_sierral_usm_cl/Documents/Documentos/Altium Designer/phoenix-c1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="838" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610783BF-7A1C-4BB5-989A-9AE1B17E1F66}"/>
+  <xr:revisionPtr revIDLastSave="852" documentId="13_ncr:1_{F7354992-1F78-49E8-A4B3-E60DEAC47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DB2FAFF-EF7E-46FE-846F-8AD6E3C6C41F}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" activeTab="2" xr2:uid="{8698A76B-EBE4-42D6-9BF9-8613B12501BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision Componentes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="250">
   <si>
     <t>power input</t>
   </si>
@@ -831,6 +831,18 @@
   </si>
   <si>
     <t>C0603 - KEMET</t>
+  </si>
+  <si>
+    <t>LPS4018-333MRC</t>
+  </si>
+  <si>
+    <t>encoder.SchDoc</t>
+  </si>
+  <si>
+    <t>leds.SchDoc</t>
+  </si>
+  <si>
+    <t>external_port.SchDoc</t>
   </si>
 </sst>
 </file>
@@ -1393,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D872604-DB61-4F0E-97E4-06141D15F6B9}">
   <dimension ref="A2:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1541,6 +1553,9 @@
       <c r="R6" t="s">
         <v>225</v>
       </c>
+      <c r="S6" t="s">
+        <v>63</v>
+      </c>
       <c r="T6" t="s">
         <v>63</v>
       </c>
@@ -1726,6 +1741,9 @@
       <c r="R10" t="s">
         <v>233</v>
       </c>
+      <c r="S10" t="s">
+        <v>63</v>
+      </c>
       <c r="T10" t="s">
         <v>63</v>
       </c>
@@ -2364,6 +2382,9 @@
       </c>
       <c r="O25" t="s">
         <v>113</v>
+      </c>
+      <c r="P25" t="s">
+        <v>246</v>
       </c>
       <c r="Q25" t="s">
         <v>63</v>
@@ -2504,6 +2525,9 @@
       </c>
       <c r="R29" t="s">
         <v>243</v>
+      </c>
+      <c r="S29" t="s">
+        <v>63</v>
       </c>
       <c r="T29" t="s">
         <v>63</v>
@@ -3256,15 +3280,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EDAD98-4A51-48B0-BAE4-039E551A8C8C}">
-  <dimension ref="B2:I40"/>
+  <dimension ref="B2:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -3714,6 +3738,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>

</xml_diff>